<commit_message>
Changes made to allwo easy analysis of expected reward.
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -257,8 +257,8 @@
   </sheetPr>
   <dimension ref="A1:T310"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A281" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S310" activeCellId="0" sqref="S310"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A274" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S308" activeCellId="0" sqref="S308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -381,11 +381,11 @@
         <v>22</v>
       </c>
       <c r="S2" s="0" t="n">
-        <f aca="false">IF(AND(R2="no", E2="tertiary"),-N2,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R2="no", E2="secondary"),-N2,0)</f>
+        <v>0</v>
       </c>
       <c r="T2" s="0" t="n">
-        <f aca="false">IF(AND(R2="yes", E2="tertiary"),11-N2,0)</f>
+        <f aca="false">IF(AND(R2="yes", E2="secondary"),11-N2,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -445,11 +445,11 @@
         <v>22</v>
       </c>
       <c r="S3" s="0" t="n">
-        <f aca="false">IF(AND(R3="no", E3="tertiary"),-N3,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R3="no", E3="secondary"),-N3,0)</f>
+        <v>-1</v>
       </c>
       <c r="T3" s="0" t="n">
-        <f aca="false">IF(AND(R3="yes", E3="tertiary"),11-N3,0)</f>
+        <f aca="false">IF(AND(R3="yes", E3="secondary"),11-N3,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -509,11 +509,11 @@
         <v>22</v>
       </c>
       <c r="S4" s="0" t="n">
-        <f aca="false">IF(AND(R4="no", E4="tertiary"),-N4,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R4="no", E4="secondary"),-N4,0)</f>
+        <v>-1</v>
       </c>
       <c r="T4" s="0" t="n">
-        <f aca="false">IF(AND(R4="yes", E4="tertiary"),11-N4,0)</f>
+        <f aca="false">IF(AND(R4="yes", E4="secondary"),11-N4,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -573,11 +573,11 @@
         <v>22</v>
       </c>
       <c r="S5" s="0" t="n">
-        <f aca="false">IF(AND(R5="no", E5="tertiary"),-N5,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R5="no", E5="secondary"),-N5,0)</f>
+        <v>0</v>
       </c>
       <c r="T5" s="0" t="n">
-        <f aca="false">IF(AND(R5="yes", E5="tertiary"),11-N5,0)</f>
+        <f aca="false">IF(AND(R5="yes", E5="secondary"),11-N5,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -637,11 +637,11 @@
         <v>22</v>
       </c>
       <c r="S6" s="0" t="n">
-        <f aca="false">IF(AND(R6="no", E6="tertiary"),-N6,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R6="no", E6="secondary"),-N6,0)</f>
+        <v>0</v>
       </c>
       <c r="T6" s="0" t="n">
-        <f aca="false">IF(AND(R6="yes", E6="tertiary"),11-N6,0)</f>
+        <f aca="false">IF(AND(R6="yes", E6="secondary"),11-N6,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -701,11 +701,11 @@
         <v>22</v>
       </c>
       <c r="S7" s="0" t="n">
-        <f aca="false">IF(AND(R7="no", E7="tertiary"),-N7,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R7="no", E7="secondary"),-N7,0)</f>
+        <v>0</v>
       </c>
       <c r="T7" s="0" t="n">
-        <f aca="false">IF(AND(R7="yes", E7="tertiary"),11-N7,0)</f>
+        <f aca="false">IF(AND(R7="yes", E7="secondary"),11-N7,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -765,11 +765,11 @@
         <v>22</v>
       </c>
       <c r="S8" s="0" t="n">
-        <f aca="false">IF(AND(R8="no", E8="tertiary"),-N8,0)</f>
+        <f aca="false">IF(AND(R8="no", E8="secondary"),-N8,0)</f>
         <v>0</v>
       </c>
       <c r="T8" s="0" t="n">
-        <f aca="false">IF(AND(R8="yes", E8="tertiary"),11-N8,0)</f>
+        <f aca="false">IF(AND(R8="yes", E8="secondary"),11-N8,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -829,11 +829,11 @@
         <v>22</v>
       </c>
       <c r="S9" s="0" t="n">
-        <f aca="false">IF(AND(R9="no", E9="tertiary"),-N9,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R9="no", E9="secondary"),-N9,0)</f>
+        <v>-1</v>
       </c>
       <c r="T9" s="0" t="n">
-        <f aca="false">IF(AND(R9="yes", E9="tertiary"),11-N9,0)</f>
+        <f aca="false">IF(AND(R9="yes", E9="secondary"),11-N9,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -893,11 +893,11 @@
         <v>22</v>
       </c>
       <c r="S10" s="0" t="n">
-        <f aca="false">IF(AND(R10="no", E10="tertiary"),-N10,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R10="no", E10="secondary"),-N10,0)</f>
+        <v>-1</v>
       </c>
       <c r="T10" s="0" t="n">
-        <f aca="false">IF(AND(R10="yes", E10="tertiary"),11-N10,0)</f>
+        <f aca="false">IF(AND(R10="yes", E10="secondary"),11-N10,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -957,11 +957,11 @@
         <v>22</v>
       </c>
       <c r="S11" s="0" t="n">
-        <f aca="false">IF(AND(R11="no", E11="tertiary"),-N11,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R11="no", E11="secondary"),-N11,0)</f>
+        <v>-1</v>
       </c>
       <c r="T11" s="0" t="n">
-        <f aca="false">IF(AND(R11="yes", E11="tertiary"),11-N11,0)</f>
+        <f aca="false">IF(AND(R11="yes", E11="secondary"),11-N11,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1021,11 +1021,11 @@
         <v>22</v>
       </c>
       <c r="S12" s="0" t="n">
-        <f aca="false">IF(AND(R12="no", E12="tertiary"),-N12,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R12="no", E12="secondary"),-N12,0)</f>
+        <v>-1</v>
       </c>
       <c r="T12" s="0" t="n">
-        <f aca="false">IF(AND(R12="yes", E12="tertiary"),11-N12,0)</f>
+        <f aca="false">IF(AND(R12="yes", E12="secondary"),11-N12,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1085,11 +1085,11 @@
         <v>22</v>
       </c>
       <c r="S13" s="0" t="n">
-        <f aca="false">IF(AND(R13="no", E13="tertiary"),-N13,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R13="no", E13="secondary"),-N13,0)</f>
+        <v>-1</v>
       </c>
       <c r="T13" s="0" t="n">
-        <f aca="false">IF(AND(R13="yes", E13="tertiary"),11-N13,0)</f>
+        <f aca="false">IF(AND(R13="yes", E13="secondary"),11-N13,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1149,11 +1149,11 @@
         <v>22</v>
       </c>
       <c r="S14" s="0" t="n">
-        <f aca="false">IF(AND(R14="no", E14="tertiary"),-N14,0)</f>
+        <f aca="false">IF(AND(R14="no", E14="secondary"),-N14,0)</f>
         <v>0</v>
       </c>
       <c r="T14" s="0" t="n">
-        <f aca="false">IF(AND(R14="yes", E14="tertiary"),11-N14,0)</f>
+        <f aca="false">IF(AND(R14="yes", E14="secondary"),11-N14,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1213,11 +1213,11 @@
         <v>22</v>
       </c>
       <c r="S15" s="0" t="n">
-        <f aca="false">IF(AND(R15="no", E15="tertiary"),-N15,0)</f>
+        <f aca="false">IF(AND(R15="no", E15="secondary"),-N15,0)</f>
         <v>0</v>
       </c>
       <c r="T15" s="0" t="n">
-        <f aca="false">IF(AND(R15="yes", E15="tertiary"),11-N15,0)</f>
+        <f aca="false">IF(AND(R15="yes", E15="secondary"),11-N15,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1277,11 +1277,11 @@
         <v>22</v>
       </c>
       <c r="S16" s="0" t="n">
-        <f aca="false">IF(AND(R16="no", E16="tertiary"),-N16,0)</f>
+        <f aca="false">IF(AND(R16="no", E16="secondary"),-N16,0)</f>
         <v>0</v>
       </c>
       <c r="T16" s="0" t="n">
-        <f aca="false">IF(AND(R16="yes", E16="tertiary"),11-N16,0)</f>
+        <f aca="false">IF(AND(R16="yes", E16="secondary"),11-N16,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1341,11 +1341,11 @@
         <v>22</v>
       </c>
       <c r="S17" s="0" t="n">
-        <f aca="false">IF(AND(R17="no", E17="tertiary"),-N17,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R17="no", E17="secondary"),-N17,0)</f>
+        <v>-1</v>
       </c>
       <c r="T17" s="0" t="n">
-        <f aca="false">IF(AND(R17="yes", E17="tertiary"),11-N17,0)</f>
+        <f aca="false">IF(AND(R17="yes", E17="secondary"),11-N17,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1405,11 +1405,11 @@
         <v>22</v>
       </c>
       <c r="S18" s="0" t="n">
-        <f aca="false">IF(AND(R18="no", E18="tertiary"),-N18,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R18="no", E18="secondary"),-N18,0)</f>
+        <v>-1</v>
       </c>
       <c r="T18" s="0" t="n">
-        <f aca="false">IF(AND(R18="yes", E18="tertiary"),11-N18,0)</f>
+        <f aca="false">IF(AND(R18="yes", E18="secondary"),11-N18,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1469,11 +1469,11 @@
         <v>22</v>
       </c>
       <c r="S19" s="0" t="n">
-        <f aca="false">IF(AND(R19="no", E19="tertiary"),-N19,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R19="no", E19="secondary"),-N19,0)</f>
+        <v>0</v>
       </c>
       <c r="T19" s="0" t="n">
-        <f aca="false">IF(AND(R19="yes", E19="tertiary"),11-N19,0)</f>
+        <f aca="false">IF(AND(R19="yes", E19="secondary"),11-N19,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1533,11 +1533,11 @@
         <v>22</v>
       </c>
       <c r="S20" s="0" t="n">
-        <f aca="false">IF(AND(R20="no", E20="tertiary"),-N20,0)</f>
+        <f aca="false">IF(AND(R20="no", E20="secondary"),-N20,0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="0" t="n">
-        <f aca="false">IF(AND(R20="yes", E20="tertiary"),11-N20,0)</f>
+        <f aca="false">IF(AND(R20="yes", E20="secondary"),11-N20,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1597,11 +1597,11 @@
         <v>22</v>
       </c>
       <c r="S21" s="0" t="n">
-        <f aca="false">IF(AND(R21="no", E21="tertiary"),-N21,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R21="no", E21="secondary"),-N21,0)</f>
+        <v>-1</v>
       </c>
       <c r="T21" s="0" t="n">
-        <f aca="false">IF(AND(R21="yes", E21="tertiary"),11-N21,0)</f>
+        <f aca="false">IF(AND(R21="yes", E21="secondary"),11-N21,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1661,11 +1661,11 @@
         <v>22</v>
       </c>
       <c r="S22" s="0" t="n">
-        <f aca="false">IF(AND(R22="no", E22="tertiary"),-N22,0)</f>
+        <f aca="false">IF(AND(R22="no", E22="secondary"),-N22,0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="0" t="n">
-        <f aca="false">IF(AND(R22="yes", E22="tertiary"),11-N22,0)</f>
+        <f aca="false">IF(AND(R22="yes", E22="secondary"),11-N22,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1725,11 +1725,11 @@
         <v>22</v>
       </c>
       <c r="S23" s="0" t="n">
-        <f aca="false">IF(AND(R23="no", E23="tertiary"),-N23,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R23="no", E23="secondary"),-N23,0)</f>
+        <v>-1</v>
       </c>
       <c r="T23" s="0" t="n">
-        <f aca="false">IF(AND(R23="yes", E23="tertiary"),11-N23,0)</f>
+        <f aca="false">IF(AND(R23="yes", E23="secondary"),11-N23,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1789,11 +1789,11 @@
         <v>22</v>
       </c>
       <c r="S24" s="0" t="n">
-        <f aca="false">IF(AND(R24="no", E24="tertiary"),-N24,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R24="no", E24="secondary"),-N24,0)</f>
+        <v>0</v>
       </c>
       <c r="T24" s="0" t="n">
-        <f aca="false">IF(AND(R24="yes", E24="tertiary"),11-N24,0)</f>
+        <f aca="false">IF(AND(R24="yes", E24="secondary"),11-N24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1853,11 +1853,11 @@
         <v>22</v>
       </c>
       <c r="S25" s="0" t="n">
-        <f aca="false">IF(AND(R25="no", E25="tertiary"),-N25,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R25="no", E25="secondary"),-N25,0)</f>
+        <v>-1</v>
       </c>
       <c r="T25" s="0" t="n">
-        <f aca="false">IF(AND(R25="yes", E25="tertiary"),11-N25,0)</f>
+        <f aca="false">IF(AND(R25="yes", E25="secondary"),11-N25,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1917,11 +1917,11 @@
         <v>22</v>
       </c>
       <c r="S26" s="0" t="n">
-        <f aca="false">IF(AND(R26="no", E26="tertiary"),-N26,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R26="no", E26="secondary"),-N26,0)</f>
+        <v>-2</v>
       </c>
       <c r="T26" s="0" t="n">
-        <f aca="false">IF(AND(R26="yes", E26="tertiary"),11-N26,0)</f>
+        <f aca="false">IF(AND(R26="yes", E26="secondary"),11-N26,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1981,11 +1981,11 @@
         <v>22</v>
       </c>
       <c r="S27" s="0" t="n">
-        <f aca="false">IF(AND(R27="no", E27="tertiary"),-N27,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R27="no", E27="secondary"),-N27,0)</f>
+        <v>-1</v>
       </c>
       <c r="T27" s="0" t="n">
-        <f aca="false">IF(AND(R27="yes", E27="tertiary"),11-N27,0)</f>
+        <f aca="false">IF(AND(R27="yes", E27="secondary"),11-N27,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2045,11 +2045,11 @@
         <v>22</v>
       </c>
       <c r="S28" s="0" t="n">
-        <f aca="false">IF(AND(R28="no", E28="tertiary"),-N28,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R28="no", E28="secondary"),-N28,0)</f>
+        <v>-1</v>
       </c>
       <c r="T28" s="0" t="n">
-        <f aca="false">IF(AND(R28="yes", E28="tertiary"),11-N28,0)</f>
+        <f aca="false">IF(AND(R28="yes", E28="secondary"),11-N28,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2109,11 +2109,11 @@
         <v>22</v>
       </c>
       <c r="S29" s="0" t="n">
-        <f aca="false">IF(AND(R29="no", E29="tertiary"),-N29,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R29="no", E29="secondary"),-N29,0)</f>
+        <v>0</v>
       </c>
       <c r="T29" s="0" t="n">
-        <f aca="false">IF(AND(R29="yes", E29="tertiary"),11-N29,0)</f>
+        <f aca="false">IF(AND(R29="yes", E29="secondary"),11-N29,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2173,11 +2173,11 @@
         <v>22</v>
       </c>
       <c r="S30" s="0" t="n">
-        <f aca="false">IF(AND(R30="no", E30="tertiary"),-N30,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R30="no", E30="secondary"),-N30,0)</f>
+        <v>-1</v>
       </c>
       <c r="T30" s="0" t="n">
-        <f aca="false">IF(AND(R30="yes", E30="tertiary"),11-N30,0)</f>
+        <f aca="false">IF(AND(R30="yes", E30="secondary"),11-N30,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2237,11 +2237,11 @@
         <v>22</v>
       </c>
       <c r="S31" s="0" t="n">
-        <f aca="false">IF(AND(R31="no", E31="tertiary"),-N31,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R31="no", E31="secondary"),-N31,0)</f>
+        <v>-1</v>
       </c>
       <c r="T31" s="0" t="n">
-        <f aca="false">IF(AND(R31="yes", E31="tertiary"),11-N31,0)</f>
+        <f aca="false">IF(AND(R31="yes", E31="secondary"),11-N31,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2301,11 +2301,11 @@
         <v>22</v>
       </c>
       <c r="S32" s="0" t="n">
-        <f aca="false">IF(AND(R32="no", E32="tertiary"),-N32,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R32="no", E32="secondary"),-N32,0)</f>
+        <v>0</v>
       </c>
       <c r="T32" s="0" t="n">
-        <f aca="false">IF(AND(R32="yes", E32="tertiary"),11-N32,0)</f>
+        <f aca="false">IF(AND(R32="yes", E32="secondary"),11-N32,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2365,11 +2365,11 @@
         <v>22</v>
       </c>
       <c r="S33" s="0" t="n">
-        <f aca="false">IF(AND(R33="no", E33="tertiary"),-N33,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R33="no", E33="secondary"),-N33,0)</f>
+        <v>-1</v>
       </c>
       <c r="T33" s="0" t="n">
-        <f aca="false">IF(AND(R33="yes", E33="tertiary"),11-N33,0)</f>
+        <f aca="false">IF(AND(R33="yes", E33="secondary"),11-N33,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2429,11 +2429,11 @@
         <v>22</v>
       </c>
       <c r="S34" s="0" t="n">
-        <f aca="false">IF(AND(R34="no", E34="tertiary"),-N34,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R34="no", E34="secondary"),-N34,0)</f>
+        <v>-1</v>
       </c>
       <c r="T34" s="0" t="n">
-        <f aca="false">IF(AND(R34="yes", E34="tertiary"),11-N34,0)</f>
+        <f aca="false">IF(AND(R34="yes", E34="secondary"),11-N34,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2493,11 +2493,11 @@
         <v>22</v>
       </c>
       <c r="S35" s="0" t="n">
-        <f aca="false">IF(AND(R35="no", E35="tertiary"),-N35,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R35="no", E35="secondary"),-N35,0)</f>
+        <v>-1</v>
       </c>
       <c r="T35" s="0" t="n">
-        <f aca="false">IF(AND(R35="yes", E35="tertiary"),11-N35,0)</f>
+        <f aca="false">IF(AND(R35="yes", E35="secondary"),11-N35,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2557,11 +2557,11 @@
         <v>22</v>
       </c>
       <c r="S36" s="0" t="n">
-        <f aca="false">IF(AND(R36="no", E36="tertiary"),-N36,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R36="no", E36="secondary"),-N36,0)</f>
+        <v>-1</v>
       </c>
       <c r="T36" s="0" t="n">
-        <f aca="false">IF(AND(R36="yes", E36="tertiary"),11-N36,0)</f>
+        <f aca="false">IF(AND(R36="yes", E36="secondary"),11-N36,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2621,11 +2621,11 @@
         <v>22</v>
       </c>
       <c r="S37" s="0" t="n">
-        <f aca="false">IF(AND(R37="no", E37="tertiary"),-N37,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R37="no", E37="secondary"),-N37,0)</f>
+        <v>-1</v>
       </c>
       <c r="T37" s="0" t="n">
-        <f aca="false">IF(AND(R37="yes", E37="tertiary"),11-N37,0)</f>
+        <f aca="false">IF(AND(R37="yes", E37="secondary"),11-N37,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2685,11 +2685,11 @@
         <v>22</v>
       </c>
       <c r="S38" s="0" t="n">
-        <f aca="false">IF(AND(R38="no", E38="tertiary"),-N38,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R38="no", E38="secondary"),-N38,0)</f>
+        <v>-1</v>
       </c>
       <c r="T38" s="0" t="n">
-        <f aca="false">IF(AND(R38="yes", E38="tertiary"),11-N38,0)</f>
+        <f aca="false">IF(AND(R38="yes", E38="secondary"),11-N38,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2749,11 +2749,11 @@
         <v>22</v>
       </c>
       <c r="S39" s="0" t="n">
-        <f aca="false">IF(AND(R39="no", E39="tertiary"),-N39,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R39="no", E39="secondary"),-N39,0)</f>
+        <v>-2</v>
       </c>
       <c r="T39" s="0" t="n">
-        <f aca="false">IF(AND(R39="yes", E39="tertiary"),11-N39,0)</f>
+        <f aca="false">IF(AND(R39="yes", E39="secondary"),11-N39,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2813,11 +2813,11 @@
         <v>22</v>
       </c>
       <c r="S40" s="0" t="n">
-        <f aca="false">IF(AND(R40="no", E40="tertiary"),-N40,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R40="no", E40="secondary"),-N40,0)</f>
+        <v>-1</v>
       </c>
       <c r="T40" s="0" t="n">
-        <f aca="false">IF(AND(R40="yes", E40="tertiary"),11-N40,0)</f>
+        <f aca="false">IF(AND(R40="yes", E40="secondary"),11-N40,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2877,11 +2877,11 @@
         <v>22</v>
       </c>
       <c r="S41" s="0" t="n">
-        <f aca="false">IF(AND(R41="no", E41="tertiary"),-N41,0)</f>
+        <f aca="false">IF(AND(R41="no", E41="secondary"),-N41,0)</f>
         <v>0</v>
       </c>
       <c r="T41" s="0" t="n">
-        <f aca="false">IF(AND(R41="yes", E41="tertiary"),11-N41,0)</f>
+        <f aca="false">IF(AND(R41="yes", E41="secondary"),11-N41,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2941,11 +2941,11 @@
         <v>22</v>
       </c>
       <c r="S42" s="0" t="n">
-        <f aca="false">IF(AND(R42="no", E42="tertiary"),-N42,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R42="no", E42="secondary"),-N42,0)</f>
+        <v>0</v>
       </c>
       <c r="T42" s="0" t="n">
-        <f aca="false">IF(AND(R42="yes", E42="tertiary"),11-N42,0)</f>
+        <f aca="false">IF(AND(R42="yes", E42="secondary"),11-N42,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3005,11 +3005,11 @@
         <v>22</v>
       </c>
       <c r="S43" s="0" t="n">
-        <f aca="false">IF(AND(R43="no", E43="tertiary"),-N43,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R43="no", E43="secondary"),-N43,0)</f>
+        <v>-2</v>
       </c>
       <c r="T43" s="0" t="n">
-        <f aca="false">IF(AND(R43="yes", E43="tertiary"),11-N43,0)</f>
+        <f aca="false">IF(AND(R43="yes", E43="secondary"),11-N43,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3069,11 +3069,11 @@
         <v>22</v>
       </c>
       <c r="S44" s="0" t="n">
-        <f aca="false">IF(AND(R44="no", E44="tertiary"),-N44,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R44="no", E44="secondary"),-N44,0)</f>
+        <v>-1</v>
       </c>
       <c r="T44" s="0" t="n">
-        <f aca="false">IF(AND(R44="yes", E44="tertiary"),11-N44,0)</f>
+        <f aca="false">IF(AND(R44="yes", E44="secondary"),11-N44,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3133,11 +3133,11 @@
         <v>22</v>
       </c>
       <c r="S45" s="0" t="n">
-        <f aca="false">IF(AND(R45="no", E45="tertiary"),-N45,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R45="no", E45="secondary"),-N45,0)</f>
+        <v>0</v>
       </c>
       <c r="T45" s="0" t="n">
-        <f aca="false">IF(AND(R45="yes", E45="tertiary"),11-N45,0)</f>
+        <f aca="false">IF(AND(R45="yes", E45="secondary"),11-N45,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3197,11 +3197,11 @@
         <v>22</v>
       </c>
       <c r="S46" s="0" t="n">
-        <f aca="false">IF(AND(R46="no", E46="tertiary"),-N46,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R46="no", E46="secondary"),-N46,0)</f>
+        <v>-1</v>
       </c>
       <c r="T46" s="0" t="n">
-        <f aca="false">IF(AND(R46="yes", E46="tertiary"),11-N46,0)</f>
+        <f aca="false">IF(AND(R46="yes", E46="secondary"),11-N46,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3261,11 +3261,11 @@
         <v>22</v>
       </c>
       <c r="S47" s="0" t="n">
-        <f aca="false">IF(AND(R47="no", E47="tertiary"),-N47,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R47="no", E47="secondary"),-N47,0)</f>
+        <v>0</v>
       </c>
       <c r="T47" s="0" t="n">
-        <f aca="false">IF(AND(R47="yes", E47="tertiary"),11-N47,0)</f>
+        <f aca="false">IF(AND(R47="yes", E47="secondary"),11-N47,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3325,11 +3325,11 @@
         <v>22</v>
       </c>
       <c r="S48" s="0" t="n">
-        <f aca="false">IF(AND(R48="no", E48="tertiary"),-N48,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R48="no", E48="secondary"),-N48,0)</f>
+        <v>0</v>
       </c>
       <c r="T48" s="0" t="n">
-        <f aca="false">IF(AND(R48="yes", E48="tertiary"),11-N48,0)</f>
+        <f aca="false">IF(AND(R48="yes", E48="secondary"),11-N48,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3389,11 +3389,11 @@
         <v>22</v>
       </c>
       <c r="S49" s="0" t="n">
-        <f aca="false">IF(AND(R49="no", E49="tertiary"),-N49,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R49="no", E49="secondary"),-N49,0)</f>
+        <v>-1</v>
       </c>
       <c r="T49" s="0" t="n">
-        <f aca="false">IF(AND(R49="yes", E49="tertiary"),11-N49,0)</f>
+        <f aca="false">IF(AND(R49="yes", E49="secondary"),11-N49,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3453,11 +3453,11 @@
         <v>22</v>
       </c>
       <c r="S50" s="0" t="n">
-        <f aca="false">IF(AND(R50="no", E50="tertiary"),-N50,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R50="no", E50="secondary"),-N50,0)</f>
+        <v>-1</v>
       </c>
       <c r="T50" s="0" t="n">
-        <f aca="false">IF(AND(R50="yes", E50="tertiary"),11-N50,0)</f>
+        <f aca="false">IF(AND(R50="yes", E50="secondary"),11-N50,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3517,11 +3517,11 @@
         <v>22</v>
       </c>
       <c r="S51" s="0" t="n">
-        <f aca="false">IF(AND(R51="no", E51="tertiary"),-N51,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R51="no", E51="secondary"),-N51,0)</f>
+        <v>0</v>
       </c>
       <c r="T51" s="0" t="n">
-        <f aca="false">IF(AND(R51="yes", E51="tertiary"),11-N51,0)</f>
+        <f aca="false">IF(AND(R51="yes", E51="secondary"),11-N51,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3581,11 +3581,11 @@
         <v>22</v>
       </c>
       <c r="S52" s="0" t="n">
-        <f aca="false">IF(AND(R52="no", E52="tertiary"),-N52,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R52="no", E52="secondary"),-N52,0)</f>
+        <v>0</v>
       </c>
       <c r="T52" s="0" t="n">
-        <f aca="false">IF(AND(R52="yes", E52="tertiary"),11-N52,0)</f>
+        <f aca="false">IF(AND(R52="yes", E52="secondary"),11-N52,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3645,11 +3645,11 @@
         <v>22</v>
       </c>
       <c r="S53" s="0" t="n">
-        <f aca="false">IF(AND(R53="no", E53="tertiary"),-N53,0)</f>
+        <f aca="false">IF(AND(R53="no", E53="secondary"),-N53,0)</f>
         <v>0</v>
       </c>
       <c r="T53" s="0" t="n">
-        <f aca="false">IF(AND(R53="yes", E53="tertiary"),11-N53,0)</f>
+        <f aca="false">IF(AND(R53="yes", E53="secondary"),11-N53,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3709,11 +3709,11 @@
         <v>22</v>
       </c>
       <c r="S54" s="0" t="n">
-        <f aca="false">IF(AND(R54="no", E54="tertiary"),-N54,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R54="no", E54="secondary"),-N54,0)</f>
+        <v>0</v>
       </c>
       <c r="T54" s="0" t="n">
-        <f aca="false">IF(AND(R54="yes", E54="tertiary"),11-N54,0)</f>
+        <f aca="false">IF(AND(R54="yes", E54="secondary"),11-N54,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3773,11 +3773,11 @@
         <v>22</v>
       </c>
       <c r="S55" s="0" t="n">
-        <f aca="false">IF(AND(R55="no", E55="tertiary"),-N55,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R55="no", E55="secondary"),-N55,0)</f>
+        <v>-1</v>
       </c>
       <c r="T55" s="0" t="n">
-        <f aca="false">IF(AND(R55="yes", E55="tertiary"),11-N55,0)</f>
+        <f aca="false">IF(AND(R55="yes", E55="secondary"),11-N55,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3837,11 +3837,11 @@
         <v>22</v>
       </c>
       <c r="S56" s="0" t="n">
-        <f aca="false">IF(AND(R56="no", E56="tertiary"),-N56,0)</f>
+        <f aca="false">IF(AND(R56="no", E56="secondary"),-N56,0)</f>
         <v>0</v>
       </c>
       <c r="T56" s="0" t="n">
-        <f aca="false">IF(AND(R56="yes", E56="tertiary"),11-N56,0)</f>
+        <f aca="false">IF(AND(R56="yes", E56="secondary"),11-N56,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3901,11 +3901,11 @@
         <v>22</v>
       </c>
       <c r="S57" s="0" t="n">
-        <f aca="false">IF(AND(R57="no", E57="tertiary"),-N57,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R57="no", E57="secondary"),-N57,0)</f>
+        <v>-1</v>
       </c>
       <c r="T57" s="0" t="n">
-        <f aca="false">IF(AND(R57="yes", E57="tertiary"),11-N57,0)</f>
+        <f aca="false">IF(AND(R57="yes", E57="secondary"),11-N57,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3965,11 +3965,11 @@
         <v>22</v>
       </c>
       <c r="S58" s="0" t="n">
-        <f aca="false">IF(AND(R58="no", E58="tertiary"),-N58,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R58="no", E58="secondary"),-N58,0)</f>
+        <v>0</v>
       </c>
       <c r="T58" s="0" t="n">
-        <f aca="false">IF(AND(R58="yes", E58="tertiary"),11-N58,0)</f>
+        <f aca="false">IF(AND(R58="yes", E58="secondary"),11-N58,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4029,11 +4029,11 @@
         <v>22</v>
       </c>
       <c r="S59" s="0" t="n">
-        <f aca="false">IF(AND(R59="no", E59="tertiary"),-N59,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R59="no", E59="secondary"),-N59,0)</f>
+        <v>0</v>
       </c>
       <c r="T59" s="0" t="n">
-        <f aca="false">IF(AND(R59="yes", E59="tertiary"),11-N59,0)</f>
+        <f aca="false">IF(AND(R59="yes", E59="secondary"),11-N59,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4093,11 +4093,11 @@
         <v>22</v>
       </c>
       <c r="S60" s="0" t="n">
-        <f aca="false">IF(AND(R60="no", E60="tertiary"),-N60,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R60="no", E60="secondary"),-N60,0)</f>
+        <v>0</v>
       </c>
       <c r="T60" s="0" t="n">
-        <f aca="false">IF(AND(R60="yes", E60="tertiary"),11-N60,0)</f>
+        <f aca="false">IF(AND(R60="yes", E60="secondary"),11-N60,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4157,11 +4157,11 @@
         <v>22</v>
       </c>
       <c r="S61" s="0" t="n">
-        <f aca="false">IF(AND(R61="no", E61="tertiary"),-N61,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R61="no", E61="secondary"),-N61,0)</f>
+        <v>-2</v>
       </c>
       <c r="T61" s="0" t="n">
-        <f aca="false">IF(AND(R61="yes", E61="tertiary"),11-N61,0)</f>
+        <f aca="false">IF(AND(R61="yes", E61="secondary"),11-N61,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4221,11 +4221,11 @@
         <v>22</v>
       </c>
       <c r="S62" s="0" t="n">
-        <f aca="false">IF(AND(R62="no", E62="tertiary"),-N62,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R62="no", E62="secondary"),-N62,0)</f>
+        <v>-1</v>
       </c>
       <c r="T62" s="0" t="n">
-        <f aca="false">IF(AND(R62="yes", E62="tertiary"),11-N62,0)</f>
+        <f aca="false">IF(AND(R62="yes", E62="secondary"),11-N62,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4285,11 +4285,11 @@
         <v>22</v>
       </c>
       <c r="S63" s="0" t="n">
-        <f aca="false">IF(AND(R63="no", E63="tertiary"),-N63,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R63="no", E63="secondary"),-N63,0)</f>
+        <v>-1</v>
       </c>
       <c r="T63" s="0" t="n">
-        <f aca="false">IF(AND(R63="yes", E63="tertiary"),11-N63,0)</f>
+        <f aca="false">IF(AND(R63="yes", E63="secondary"),11-N63,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4349,11 +4349,11 @@
         <v>22</v>
       </c>
       <c r="S64" s="0" t="n">
-        <f aca="false">IF(AND(R64="no", E64="tertiary"),-N64,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R64="no", E64="secondary"),-N64,0)</f>
+        <v>-1</v>
       </c>
       <c r="T64" s="0" t="n">
-        <f aca="false">IF(AND(R64="yes", E64="tertiary"),11-N64,0)</f>
+        <f aca="false">IF(AND(R64="yes", E64="secondary"),11-N64,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4413,11 +4413,11 @@
         <v>22</v>
       </c>
       <c r="S65" s="0" t="n">
-        <f aca="false">IF(AND(R65="no", E65="tertiary"),-N65,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R65="no", E65="secondary"),-N65,0)</f>
+        <v>-1</v>
       </c>
       <c r="T65" s="0" t="n">
-        <f aca="false">IF(AND(R65="yes", E65="tertiary"),11-N65,0)</f>
+        <f aca="false">IF(AND(R65="yes", E65="secondary"),11-N65,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4477,11 +4477,11 @@
         <v>22</v>
       </c>
       <c r="S66" s="0" t="n">
-        <f aca="false">IF(AND(R66="no", E66="tertiary"),-N66,0)</f>
+        <f aca="false">IF(AND(R66="no", E66="secondary"),-N66,0)</f>
         <v>0</v>
       </c>
       <c r="T66" s="0" t="n">
-        <f aca="false">IF(AND(R66="yes", E66="tertiary"),11-N66,0)</f>
+        <f aca="false">IF(AND(R66="yes", E66="secondary"),11-N66,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4541,11 +4541,11 @@
         <v>22</v>
       </c>
       <c r="S67" s="0" t="n">
-        <f aca="false">IF(AND(R67="no", E67="tertiary"),-N67,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R67="no", E67="secondary"),-N67,0)</f>
+        <v>-1</v>
       </c>
       <c r="T67" s="0" t="n">
-        <f aca="false">IF(AND(R67="yes", E67="tertiary"),11-N67,0)</f>
+        <f aca="false">IF(AND(R67="yes", E67="secondary"),11-N67,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4605,11 +4605,11 @@
         <v>22</v>
       </c>
       <c r="S68" s="0" t="n">
-        <f aca="false">IF(AND(R68="no", E68="tertiary"),-N68,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R68="no", E68="secondary"),-N68,0)</f>
+        <v>-1</v>
       </c>
       <c r="T68" s="0" t="n">
-        <f aca="false">IF(AND(R68="yes", E68="tertiary"),11-N68,0)</f>
+        <f aca="false">IF(AND(R68="yes", E68="secondary"),11-N68,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4669,11 +4669,11 @@
         <v>22</v>
       </c>
       <c r="S69" s="0" t="n">
-        <f aca="false">IF(AND(R69="no", E69="tertiary"),-N69,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R69="no", E69="secondary"),-N69,0)</f>
+        <v>-1</v>
       </c>
       <c r="T69" s="0" t="n">
-        <f aca="false">IF(AND(R69="yes", E69="tertiary"),11-N69,0)</f>
+        <f aca="false">IF(AND(R69="yes", E69="secondary"),11-N69,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4733,11 +4733,11 @@
         <v>22</v>
       </c>
       <c r="S70" s="0" t="n">
-        <f aca="false">IF(AND(R70="no", E70="tertiary"),-N70,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R70="no", E70="secondary"),-N70,0)</f>
+        <v>-1</v>
       </c>
       <c r="T70" s="0" t="n">
-        <f aca="false">IF(AND(R70="yes", E70="tertiary"),11-N70,0)</f>
+        <f aca="false">IF(AND(R70="yes", E70="secondary"),11-N70,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4797,11 +4797,11 @@
         <v>22</v>
       </c>
       <c r="S71" s="0" t="n">
-        <f aca="false">IF(AND(R71="no", E71="tertiary"),-N71,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R71="no", E71="secondary"),-N71,0)</f>
+        <v>-1</v>
       </c>
       <c r="T71" s="0" t="n">
-        <f aca="false">IF(AND(R71="yes", E71="tertiary"),11-N71,0)</f>
+        <f aca="false">IF(AND(R71="yes", E71="secondary"),11-N71,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4861,11 +4861,11 @@
         <v>22</v>
       </c>
       <c r="S72" s="0" t="n">
-        <f aca="false">IF(AND(R72="no", E72="tertiary"),-N72,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R72="no", E72="secondary"),-N72,0)</f>
+        <v>-1</v>
       </c>
       <c r="T72" s="0" t="n">
-        <f aca="false">IF(AND(R72="yes", E72="tertiary"),11-N72,0)</f>
+        <f aca="false">IF(AND(R72="yes", E72="secondary"),11-N72,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4925,11 +4925,11 @@
         <v>22</v>
       </c>
       <c r="S73" s="0" t="n">
-        <f aca="false">IF(AND(R73="no", E73="tertiary"),-N73,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R73="no", E73="secondary"),-N73,0)</f>
+        <v>-1</v>
       </c>
       <c r="T73" s="0" t="n">
-        <f aca="false">IF(AND(R73="yes", E73="tertiary"),11-N73,0)</f>
+        <f aca="false">IF(AND(R73="yes", E73="secondary"),11-N73,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4989,11 +4989,11 @@
         <v>22</v>
       </c>
       <c r="S74" s="0" t="n">
-        <f aca="false">IF(AND(R74="no", E74="tertiary"),-N74,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R74="no", E74="secondary"),-N74,0)</f>
+        <v>-1</v>
       </c>
       <c r="T74" s="0" t="n">
-        <f aca="false">IF(AND(R74="yes", E74="tertiary"),11-N74,0)</f>
+        <f aca="false">IF(AND(R74="yes", E74="secondary"),11-N74,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5053,11 +5053,11 @@
         <v>22</v>
       </c>
       <c r="S75" s="0" t="n">
-        <f aca="false">IF(AND(R75="no", E75="tertiary"),-N75,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R75="no", E75="secondary"),-N75,0)</f>
+        <v>-1</v>
       </c>
       <c r="T75" s="0" t="n">
-        <f aca="false">IF(AND(R75="yes", E75="tertiary"),11-N75,0)</f>
+        <f aca="false">IF(AND(R75="yes", E75="secondary"),11-N75,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5117,12 +5117,12 @@
         <v>23</v>
       </c>
       <c r="S76" s="0" t="n">
-        <f aca="false">IF(AND(R76="no", E76="tertiary"),-N76,0)</f>
+        <f aca="false">IF(AND(R76="no", E76="secondary"),-N76,0)</f>
         <v>0</v>
       </c>
       <c r="T76" s="0" t="n">
-        <f aca="false">IF(AND(R76="yes", E76="tertiary"),11-N76,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R76="yes", E76="secondary"),11-N76,0)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5181,11 +5181,11 @@
         <v>22</v>
       </c>
       <c r="S77" s="0" t="n">
-        <f aca="false">IF(AND(R77="no", E77="tertiary"),-N77,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R77="no", E77="secondary"),-N77,0)</f>
+        <v>0</v>
       </c>
       <c r="T77" s="0" t="n">
-        <f aca="false">IF(AND(R77="yes", E77="tertiary"),11-N77,0)</f>
+        <f aca="false">IF(AND(R77="yes", E77="secondary"),11-N77,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5245,11 +5245,11 @@
         <v>22</v>
       </c>
       <c r="S78" s="0" t="n">
-        <f aca="false">IF(AND(R78="no", E78="tertiary"),-N78,0)</f>
+        <f aca="false">IF(AND(R78="no", E78="secondary"),-N78,0)</f>
         <v>0</v>
       </c>
       <c r="T78" s="0" t="n">
-        <f aca="false">IF(AND(R78="yes", E78="tertiary"),11-N78,0)</f>
+        <f aca="false">IF(AND(R78="yes", E78="secondary"),11-N78,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5309,12 +5309,12 @@
         <v>23</v>
       </c>
       <c r="S79" s="0" t="n">
-        <f aca="false">IF(AND(R79="no", E79="tertiary"),-N79,0)</f>
+        <f aca="false">IF(AND(R79="no", E79="secondary"),-N79,0)</f>
         <v>0</v>
       </c>
       <c r="T79" s="0" t="n">
-        <f aca="false">IF(AND(R79="yes", E79="tertiary"),11-N79,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R79="yes", E79="secondary"),11-N79,0)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5373,12 +5373,12 @@
         <v>23</v>
       </c>
       <c r="S80" s="0" t="n">
-        <f aca="false">IF(AND(R80="no", E80="tertiary"),-N80,0)</f>
+        <f aca="false">IF(AND(R80="no", E80="secondary"),-N80,0)</f>
         <v>0</v>
       </c>
       <c r="T80" s="0" t="n">
-        <f aca="false">IF(AND(R80="yes", E80="tertiary"),11-N80,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R80="yes", E80="secondary"),11-N80,0)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5437,11 +5437,11 @@
         <v>22</v>
       </c>
       <c r="S81" s="0" t="n">
-        <f aca="false">IF(AND(R81="no", E81="tertiary"),-N81,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R81="no", E81="secondary"),-N81,0)</f>
+        <v>-2</v>
       </c>
       <c r="T81" s="0" t="n">
-        <f aca="false">IF(AND(R81="yes", E81="tertiary"),11-N81,0)</f>
+        <f aca="false">IF(AND(R81="yes", E81="secondary"),11-N81,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5501,11 +5501,11 @@
         <v>22</v>
       </c>
       <c r="S82" s="0" t="n">
-        <f aca="false">IF(AND(R82="no", E82="tertiary"),-N82,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R82="no", E82="secondary"),-N82,0)</f>
+        <v>-2</v>
       </c>
       <c r="T82" s="0" t="n">
-        <f aca="false">IF(AND(R82="yes", E82="tertiary"),11-N82,0)</f>
+        <f aca="false">IF(AND(R82="yes", E82="secondary"),11-N82,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5565,11 +5565,11 @@
         <v>22</v>
       </c>
       <c r="S83" s="0" t="n">
-        <f aca="false">IF(AND(R83="no", E83="tertiary"),-N83,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R83="no", E83="secondary"),-N83,0)</f>
+        <v>-1</v>
       </c>
       <c r="T83" s="0" t="n">
-        <f aca="false">IF(AND(R83="yes", E83="tertiary"),11-N83,0)</f>
+        <f aca="false">IF(AND(R83="yes", E83="secondary"),11-N83,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5629,11 +5629,11 @@
         <v>22</v>
       </c>
       <c r="S84" s="0" t="n">
-        <f aca="false">IF(AND(R84="no", E84="tertiary"),-N84,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R84="no", E84="secondary"),-N84,0)</f>
+        <v>-2</v>
       </c>
       <c r="T84" s="0" t="n">
-        <f aca="false">IF(AND(R84="yes", E84="tertiary"),11-N84,0)</f>
+        <f aca="false">IF(AND(R84="yes", E84="secondary"),11-N84,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5693,11 +5693,11 @@
         <v>22</v>
       </c>
       <c r="S85" s="0" t="n">
-        <f aca="false">IF(AND(R85="no", E85="tertiary"),-N85,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R85="no", E85="secondary"),-N85,0)</f>
+        <v>-1</v>
       </c>
       <c r="T85" s="0" t="n">
-        <f aca="false">IF(AND(R85="yes", E85="tertiary"),11-N85,0)</f>
+        <f aca="false">IF(AND(R85="yes", E85="secondary"),11-N85,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5757,11 +5757,11 @@
         <v>22</v>
       </c>
       <c r="S86" s="0" t="n">
-        <f aca="false">IF(AND(R86="no", E86="tertiary"),-N86,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R86="no", E86="secondary"),-N86,0)</f>
+        <v>-1</v>
       </c>
       <c r="T86" s="0" t="n">
-        <f aca="false">IF(AND(R86="yes", E86="tertiary"),11-N86,0)</f>
+        <f aca="false">IF(AND(R86="yes", E86="secondary"),11-N86,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5821,11 +5821,11 @@
         <v>22</v>
       </c>
       <c r="S87" s="0" t="n">
-        <f aca="false">IF(AND(R87="no", E87="tertiary"),-N87,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R87="no", E87="secondary"),-N87,0)</f>
+        <v>0</v>
       </c>
       <c r="T87" s="0" t="n">
-        <f aca="false">IF(AND(R87="yes", E87="tertiary"),11-N87,0)</f>
+        <f aca="false">IF(AND(R87="yes", E87="secondary"),11-N87,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5885,11 +5885,11 @@
         <v>22</v>
       </c>
       <c r="S88" s="0" t="n">
-        <f aca="false">IF(AND(R88="no", E88="tertiary"),-N88,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R88="no", E88="secondary"),-N88,0)</f>
+        <v>-1</v>
       </c>
       <c r="T88" s="0" t="n">
-        <f aca="false">IF(AND(R88="yes", E88="tertiary"),11-N88,0)</f>
+        <f aca="false">IF(AND(R88="yes", E88="secondary"),11-N88,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5949,11 +5949,11 @@
         <v>22</v>
       </c>
       <c r="S89" s="0" t="n">
-        <f aca="false">IF(AND(R89="no", E89="tertiary"),-N89,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R89="no", E89="secondary"),-N89,0)</f>
+        <v>0</v>
       </c>
       <c r="T89" s="0" t="n">
-        <f aca="false">IF(AND(R89="yes", E89="tertiary"),11-N89,0)</f>
+        <f aca="false">IF(AND(R89="yes", E89="secondary"),11-N89,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6013,11 +6013,11 @@
         <v>22</v>
       </c>
       <c r="S90" s="0" t="n">
-        <f aca="false">IF(AND(R90="no", E90="tertiary"),-N90,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R90="no", E90="secondary"),-N90,0)</f>
+        <v>-1</v>
       </c>
       <c r="T90" s="0" t="n">
-        <f aca="false">IF(AND(R90="yes", E90="tertiary"),11-N90,0)</f>
+        <f aca="false">IF(AND(R90="yes", E90="secondary"),11-N90,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6077,11 +6077,11 @@
         <v>22</v>
       </c>
       <c r="S91" s="0" t="n">
-        <f aca="false">IF(AND(R91="no", E91="tertiary"),-N91,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R91="no", E91="secondary"),-N91,0)</f>
+        <v>0</v>
       </c>
       <c r="T91" s="0" t="n">
-        <f aca="false">IF(AND(R91="yes", E91="tertiary"),11-N91,0)</f>
+        <f aca="false">IF(AND(R91="yes", E91="secondary"),11-N91,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6141,11 +6141,11 @@
         <v>22</v>
       </c>
       <c r="S92" s="0" t="n">
-        <f aca="false">IF(AND(R92="no", E92="tertiary"),-N92,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R92="no", E92="secondary"),-N92,0)</f>
+        <v>-1</v>
       </c>
       <c r="T92" s="0" t="n">
-        <f aca="false">IF(AND(R92="yes", E92="tertiary"),11-N92,0)</f>
+        <f aca="false">IF(AND(R92="yes", E92="secondary"),11-N92,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6205,11 +6205,11 @@
         <v>22</v>
       </c>
       <c r="S93" s="0" t="n">
-        <f aca="false">IF(AND(R93="no", E93="tertiary"),-N93,0)</f>
+        <f aca="false">IF(AND(R93="no", E93="secondary"),-N93,0)</f>
         <v>0</v>
       </c>
       <c r="T93" s="0" t="n">
-        <f aca="false">IF(AND(R93="yes", E93="tertiary"),11-N93,0)</f>
+        <f aca="false">IF(AND(R93="yes", E93="secondary"),11-N93,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6269,11 +6269,11 @@
         <v>22</v>
       </c>
       <c r="S94" s="0" t="n">
-        <f aca="false">IF(AND(R94="no", E94="tertiary"),-N94,0)</f>
+        <f aca="false">IF(AND(R94="no", E94="secondary"),-N94,0)</f>
         <v>0</v>
       </c>
       <c r="T94" s="0" t="n">
-        <f aca="false">IF(AND(R94="yes", E94="tertiary"),11-N94,0)</f>
+        <f aca="false">IF(AND(R94="yes", E94="secondary"),11-N94,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6333,11 +6333,11 @@
         <v>22</v>
       </c>
       <c r="S95" s="0" t="n">
-        <f aca="false">IF(AND(R95="no", E95="tertiary"),-N95,0)</f>
+        <f aca="false">IF(AND(R95="no", E95="secondary"),-N95,0)</f>
         <v>0</v>
       </c>
       <c r="T95" s="0" t="n">
-        <f aca="false">IF(AND(R95="yes", E95="tertiary"),11-N95,0)</f>
+        <f aca="false">IF(AND(R95="yes", E95="secondary"),11-N95,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6397,11 +6397,11 @@
         <v>22</v>
       </c>
       <c r="S96" s="0" t="n">
-        <f aca="false">IF(AND(R96="no", E96="tertiary"),-N96,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R96="no", E96="secondary"),-N96,0)</f>
+        <v>0</v>
       </c>
       <c r="T96" s="0" t="n">
-        <f aca="false">IF(AND(R96="yes", E96="tertiary"),11-N96,0)</f>
+        <f aca="false">IF(AND(R96="yes", E96="secondary"),11-N96,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6461,11 +6461,11 @@
         <v>22</v>
       </c>
       <c r="S97" s="0" t="n">
-        <f aca="false">IF(AND(R97="no", E97="tertiary"),-N97,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R97="no", E97="secondary"),-N97,0)</f>
+        <v>-1</v>
       </c>
       <c r="T97" s="0" t="n">
-        <f aca="false">IF(AND(R97="yes", E97="tertiary"),11-N97,0)</f>
+        <f aca="false">IF(AND(R97="yes", E97="secondary"),11-N97,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6525,11 +6525,11 @@
         <v>22</v>
       </c>
       <c r="S98" s="0" t="n">
-        <f aca="false">IF(AND(R98="no", E98="tertiary"),-N98,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R98="no", E98="secondary"),-N98,0)</f>
+        <v>0</v>
       </c>
       <c r="T98" s="0" t="n">
-        <f aca="false">IF(AND(R98="yes", E98="tertiary"),11-N98,0)</f>
+        <f aca="false">IF(AND(R98="yes", E98="secondary"),11-N98,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6589,11 +6589,11 @@
         <v>22</v>
       </c>
       <c r="S99" s="0" t="n">
-        <f aca="false">IF(AND(R99="no", E99="tertiary"),-N99,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R99="no", E99="secondary"),-N99,0)</f>
+        <v>-1</v>
       </c>
       <c r="T99" s="0" t="n">
-        <f aca="false">IF(AND(R99="yes", E99="tertiary"),11-N99,0)</f>
+        <f aca="false">IF(AND(R99="yes", E99="secondary"),11-N99,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6653,11 +6653,11 @@
         <v>22</v>
       </c>
       <c r="S100" s="0" t="n">
-        <f aca="false">IF(AND(R100="no", E100="tertiary"),-N100,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R100="no", E100="secondary"),-N100,0)</f>
+        <v>-1</v>
       </c>
       <c r="T100" s="0" t="n">
-        <f aca="false">IF(AND(R100="yes", E100="tertiary"),11-N100,0)</f>
+        <f aca="false">IF(AND(R100="yes", E100="secondary"),11-N100,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6717,11 +6717,11 @@
         <v>22</v>
       </c>
       <c r="S101" s="0" t="n">
-        <f aca="false">IF(AND(R101="no", E101="tertiary"),-N101,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R101="no", E101="secondary"),-N101,0)</f>
+        <v>0</v>
       </c>
       <c r="T101" s="0" t="n">
-        <f aca="false">IF(AND(R101="yes", E101="tertiary"),11-N101,0)</f>
+        <f aca="false">IF(AND(R101="yes", E101="secondary"),11-N101,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6781,11 +6781,11 @@
         <v>22</v>
       </c>
       <c r="S102" s="0" t="n">
-        <f aca="false">IF(AND(R102="no", E102="tertiary"),-N102,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R102="no", E102="secondary"),-N102,0)</f>
+        <v>-1</v>
       </c>
       <c r="T102" s="0" t="n">
-        <f aca="false">IF(AND(R102="yes", E102="tertiary"),11-N102,0)</f>
+        <f aca="false">IF(AND(R102="yes", E102="secondary"),11-N102,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6845,11 +6845,11 @@
         <v>22</v>
       </c>
       <c r="S103" s="0" t="n">
-        <f aca="false">IF(AND(R103="no", E103="tertiary"),-N103,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R103="no", E103="secondary"),-N103,0)</f>
+        <v>-1</v>
       </c>
       <c r="T103" s="0" t="n">
-        <f aca="false">IF(AND(R103="yes", E103="tertiary"),11-N103,0)</f>
+        <f aca="false">IF(AND(R103="yes", E103="secondary"),11-N103,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6909,11 +6909,11 @@
         <v>22</v>
       </c>
       <c r="S104" s="0" t="n">
-        <f aca="false">IF(AND(R104="no", E104="tertiary"),-N104,0)</f>
+        <f aca="false">IF(AND(R104="no", E104="secondary"),-N104,0)</f>
         <v>0</v>
       </c>
       <c r="T104" s="0" t="n">
-        <f aca="false">IF(AND(R104="yes", E104="tertiary"),11-N104,0)</f>
+        <f aca="false">IF(AND(R104="yes", E104="secondary"),11-N104,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6973,11 +6973,11 @@
         <v>22</v>
       </c>
       <c r="S105" s="0" t="n">
-        <f aca="false">IF(AND(R105="no", E105="tertiary"),-N105,0)</f>
+        <f aca="false">IF(AND(R105="no", E105="secondary"),-N105,0)</f>
         <v>0</v>
       </c>
       <c r="T105" s="0" t="n">
-        <f aca="false">IF(AND(R105="yes", E105="tertiary"),11-N105,0)</f>
+        <f aca="false">IF(AND(R105="yes", E105="secondary"),11-N105,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7037,11 +7037,11 @@
         <v>22</v>
       </c>
       <c r="S106" s="0" t="n">
-        <f aca="false">IF(AND(R106="no", E106="tertiary"),-N106,0)</f>
+        <f aca="false">IF(AND(R106="no", E106="secondary"),-N106,0)</f>
         <v>0</v>
       </c>
       <c r="T106" s="0" t="n">
-        <f aca="false">IF(AND(R106="yes", E106="tertiary"),11-N106,0)</f>
+        <f aca="false">IF(AND(R106="yes", E106="secondary"),11-N106,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7101,11 +7101,11 @@
         <v>22</v>
       </c>
       <c r="S107" s="0" t="n">
-        <f aca="false">IF(AND(R107="no", E107="tertiary"),-N107,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R107="no", E107="secondary"),-N107,0)</f>
+        <v>-2</v>
       </c>
       <c r="T107" s="0" t="n">
-        <f aca="false">IF(AND(R107="yes", E107="tertiary"),11-N107,0)</f>
+        <f aca="false">IF(AND(R107="yes", E107="secondary"),11-N107,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7165,11 +7165,11 @@
         <v>22</v>
       </c>
       <c r="S108" s="0" t="n">
-        <f aca="false">IF(AND(R108="no", E108="tertiary"),-N108,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R108="no", E108="secondary"),-N108,0)</f>
+        <v>-1</v>
       </c>
       <c r="T108" s="0" t="n">
-        <f aca="false">IF(AND(R108="yes", E108="tertiary"),11-N108,0)</f>
+        <f aca="false">IF(AND(R108="yes", E108="secondary"),11-N108,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7229,11 +7229,11 @@
         <v>22</v>
       </c>
       <c r="S109" s="0" t="n">
-        <f aca="false">IF(AND(R109="no", E109="tertiary"),-N109,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R109="no", E109="secondary"),-N109,0)</f>
+        <v>0</v>
       </c>
       <c r="T109" s="0" t="n">
-        <f aca="false">IF(AND(R109="yes", E109="tertiary"),11-N109,0)</f>
+        <f aca="false">IF(AND(R109="yes", E109="secondary"),11-N109,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7293,11 +7293,11 @@
         <v>22</v>
       </c>
       <c r="S110" s="0" t="n">
-        <f aca="false">IF(AND(R110="no", E110="tertiary"),-N110,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R110="no", E110="secondary"),-N110,0)</f>
+        <v>0</v>
       </c>
       <c r="T110" s="0" t="n">
-        <f aca="false">IF(AND(R110="yes", E110="tertiary"),11-N110,0)</f>
+        <f aca="false">IF(AND(R110="yes", E110="secondary"),11-N110,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7357,11 +7357,11 @@
         <v>22</v>
       </c>
       <c r="S111" s="0" t="n">
-        <f aca="false">IF(AND(R111="no", E111="tertiary"),-N111,0)</f>
+        <f aca="false">IF(AND(R111="no", E111="secondary"),-N111,0)</f>
         <v>0</v>
       </c>
       <c r="T111" s="0" t="n">
-        <f aca="false">IF(AND(R111="yes", E111="tertiary"),11-N111,0)</f>
+        <f aca="false">IF(AND(R111="yes", E111="secondary"),11-N111,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7421,11 +7421,11 @@
         <v>22</v>
       </c>
       <c r="S112" s="0" t="n">
-        <f aca="false">IF(AND(R112="no", E112="tertiary"),-N112,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R112="no", E112="secondary"),-N112,0)</f>
+        <v>-1</v>
       </c>
       <c r="T112" s="0" t="n">
-        <f aca="false">IF(AND(R112="yes", E112="tertiary"),11-N112,0)</f>
+        <f aca="false">IF(AND(R112="yes", E112="secondary"),11-N112,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7485,11 +7485,11 @@
         <v>22</v>
       </c>
       <c r="S113" s="0" t="n">
-        <f aca="false">IF(AND(R113="no", E113="tertiary"),-N113,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R113="no", E113="secondary"),-N113,0)</f>
+        <v>-2</v>
       </c>
       <c r="T113" s="0" t="n">
-        <f aca="false">IF(AND(R113="yes", E113="tertiary"),11-N113,0)</f>
+        <f aca="false">IF(AND(R113="yes", E113="secondary"),11-N113,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7549,11 +7549,11 @@
         <v>22</v>
       </c>
       <c r="S114" s="0" t="n">
-        <f aca="false">IF(AND(R114="no", E114="tertiary"),-N114,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R114="no", E114="secondary"),-N114,0)</f>
+        <v>0</v>
       </c>
       <c r="T114" s="0" t="n">
-        <f aca="false">IF(AND(R114="yes", E114="tertiary"),11-N114,0)</f>
+        <f aca="false">IF(AND(R114="yes", E114="secondary"),11-N114,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7613,11 +7613,11 @@
         <v>22</v>
       </c>
       <c r="S115" s="0" t="n">
-        <f aca="false">IF(AND(R115="no", E115="tertiary"),-N115,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R115="no", E115="secondary"),-N115,0)</f>
+        <v>-2</v>
       </c>
       <c r="T115" s="0" t="n">
-        <f aca="false">IF(AND(R115="yes", E115="tertiary"),11-N115,0)</f>
+        <f aca="false">IF(AND(R115="yes", E115="secondary"),11-N115,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7677,11 +7677,11 @@
         <v>22</v>
       </c>
       <c r="S116" s="0" t="n">
-        <f aca="false">IF(AND(R116="no", E116="tertiary"),-N116,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R116="no", E116="secondary"),-N116,0)</f>
+        <v>-1</v>
       </c>
       <c r="T116" s="0" t="n">
-        <f aca="false">IF(AND(R116="yes", E116="tertiary"),11-N116,0)</f>
+        <f aca="false">IF(AND(R116="yes", E116="secondary"),11-N116,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7741,11 +7741,11 @@
         <v>22</v>
       </c>
       <c r="S117" s="0" t="n">
-        <f aca="false">IF(AND(R117="no", E117="tertiary"),-N117,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R117="no", E117="secondary"),-N117,0)</f>
+        <v>-1</v>
       </c>
       <c r="T117" s="0" t="n">
-        <f aca="false">IF(AND(R117="yes", E117="tertiary"),11-N117,0)</f>
+        <f aca="false">IF(AND(R117="yes", E117="secondary"),11-N117,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7805,11 +7805,11 @@
         <v>22</v>
       </c>
       <c r="S118" s="0" t="n">
-        <f aca="false">IF(AND(R118="no", E118="tertiary"),-N118,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R118="no", E118="secondary"),-N118,0)</f>
+        <v>-1</v>
       </c>
       <c r="T118" s="0" t="n">
-        <f aca="false">IF(AND(R118="yes", E118="tertiary"),11-N118,0)</f>
+        <f aca="false">IF(AND(R118="yes", E118="secondary"),11-N118,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7869,12 +7869,12 @@
         <v>23</v>
       </c>
       <c r="S119" s="0" t="n">
-        <f aca="false">IF(AND(R119="no", E119="tertiary"),-N119,0)</f>
+        <f aca="false">IF(AND(R119="no", E119="secondary"),-N119,0)</f>
         <v>0</v>
       </c>
       <c r="T119" s="0" t="n">
-        <f aca="false">IF(AND(R119="yes", E119="tertiary"),11-N119,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R119="yes", E119="secondary"),11-N119,0)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7933,11 +7933,11 @@
         <v>22</v>
       </c>
       <c r="S120" s="0" t="n">
-        <f aca="false">IF(AND(R120="no", E120="tertiary"),-N120,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R120="no", E120="secondary"),-N120,0)</f>
+        <v>-1</v>
       </c>
       <c r="T120" s="0" t="n">
-        <f aca="false">IF(AND(R120="yes", E120="tertiary"),11-N120,0)</f>
+        <f aca="false">IF(AND(R120="yes", E120="secondary"),11-N120,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7997,11 +7997,11 @@
         <v>22</v>
       </c>
       <c r="S121" s="0" t="n">
-        <f aca="false">IF(AND(R121="no", E121="tertiary"),-N121,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R121="no", E121="secondary"),-N121,0)</f>
+        <v>-1</v>
       </c>
       <c r="T121" s="0" t="n">
-        <f aca="false">IF(AND(R121="yes", E121="tertiary"),11-N121,0)</f>
+        <f aca="false">IF(AND(R121="yes", E121="secondary"),11-N121,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8061,11 +8061,11 @@
         <v>22</v>
       </c>
       <c r="S122" s="0" t="n">
-        <f aca="false">IF(AND(R122="no", E122="tertiary"),-N122,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R122="no", E122="secondary"),-N122,0)</f>
+        <v>-2</v>
       </c>
       <c r="T122" s="0" t="n">
-        <f aca="false">IF(AND(R122="yes", E122="tertiary"),11-N122,0)</f>
+        <f aca="false">IF(AND(R122="yes", E122="secondary"),11-N122,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8125,11 +8125,11 @@
         <v>22</v>
       </c>
       <c r="S123" s="0" t="n">
-        <f aca="false">IF(AND(R123="no", E123="tertiary"),-N123,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R123="no", E123="secondary"),-N123,0)</f>
+        <v>0</v>
       </c>
       <c r="T123" s="0" t="n">
-        <f aca="false">IF(AND(R123="yes", E123="tertiary"),11-N123,0)</f>
+        <f aca="false">IF(AND(R123="yes", E123="secondary"),11-N123,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8189,11 +8189,11 @@
         <v>22</v>
       </c>
       <c r="S124" s="0" t="n">
-        <f aca="false">IF(AND(R124="no", E124="tertiary"),-N124,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R124="no", E124="secondary"),-N124,0)</f>
+        <v>-1</v>
       </c>
       <c r="T124" s="0" t="n">
-        <f aca="false">IF(AND(R124="yes", E124="tertiary"),11-N124,0)</f>
+        <f aca="false">IF(AND(R124="yes", E124="secondary"),11-N124,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8253,11 +8253,11 @@
         <v>22</v>
       </c>
       <c r="S125" s="0" t="n">
-        <f aca="false">IF(AND(R125="no", E125="tertiary"),-N125,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R125="no", E125="secondary"),-N125,0)</f>
+        <v>-1</v>
       </c>
       <c r="T125" s="0" t="n">
-        <f aca="false">IF(AND(R125="yes", E125="tertiary"),11-N125,0)</f>
+        <f aca="false">IF(AND(R125="yes", E125="secondary"),11-N125,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8317,11 +8317,11 @@
         <v>22</v>
       </c>
       <c r="S126" s="0" t="n">
-        <f aca="false">IF(AND(R126="no", E126="tertiary"),-N126,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R126="no", E126="secondary"),-N126,0)</f>
+        <v>-1</v>
       </c>
       <c r="T126" s="0" t="n">
-        <f aca="false">IF(AND(R126="yes", E126="tertiary"),11-N126,0)</f>
+        <f aca="false">IF(AND(R126="yes", E126="secondary"),11-N126,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8381,11 +8381,11 @@
         <v>22</v>
       </c>
       <c r="S127" s="0" t="n">
-        <f aca="false">IF(AND(R127="no", E127="tertiary"),-N127,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R127="no", E127="secondary"),-N127,0)</f>
+        <v>-1</v>
       </c>
       <c r="T127" s="0" t="n">
-        <f aca="false">IF(AND(R127="yes", E127="tertiary"),11-N127,0)</f>
+        <f aca="false">IF(AND(R127="yes", E127="secondary"),11-N127,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8445,11 +8445,11 @@
         <v>22</v>
       </c>
       <c r="S128" s="0" t="n">
-        <f aca="false">IF(AND(R128="no", E128="tertiary"),-N128,0)</f>
+        <f aca="false">IF(AND(R128="no", E128="secondary"),-N128,0)</f>
         <v>0</v>
       </c>
       <c r="T128" s="0" t="n">
-        <f aca="false">IF(AND(R128="yes", E128="tertiary"),11-N128,0)</f>
+        <f aca="false">IF(AND(R128="yes", E128="secondary"),11-N128,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8509,11 +8509,11 @@
         <v>22</v>
       </c>
       <c r="S129" s="0" t="n">
-        <f aca="false">IF(AND(R129="no", E129="tertiary"),-N129,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R129="no", E129="secondary"),-N129,0)</f>
+        <v>-1</v>
       </c>
       <c r="T129" s="0" t="n">
-        <f aca="false">IF(AND(R129="yes", E129="tertiary"),11-N129,0)</f>
+        <f aca="false">IF(AND(R129="yes", E129="secondary"),11-N129,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8573,11 +8573,11 @@
         <v>22</v>
       </c>
       <c r="S130" s="0" t="n">
-        <f aca="false">IF(AND(R130="no", E130="tertiary"),-N130,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R130="no", E130="secondary"),-N130,0)</f>
+        <v>0</v>
       </c>
       <c r="T130" s="0" t="n">
-        <f aca="false">IF(AND(R130="yes", E130="tertiary"),11-N130,0)</f>
+        <f aca="false">IF(AND(R130="yes", E130="secondary"),11-N130,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8637,11 +8637,11 @@
         <v>22</v>
       </c>
       <c r="S131" s="0" t="n">
-        <f aca="false">IF(AND(R131="no", E131="tertiary"),-N131,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R131="no", E131="secondary"),-N131,0)</f>
+        <v>-1</v>
       </c>
       <c r="T131" s="0" t="n">
-        <f aca="false">IF(AND(R131="yes", E131="tertiary"),11-N131,0)</f>
+        <f aca="false">IF(AND(R131="yes", E131="secondary"),11-N131,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8701,11 +8701,11 @@
         <v>22</v>
       </c>
       <c r="S132" s="0" t="n">
-        <f aca="false">IF(AND(R132="no", E132="tertiary"),-N132,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R132="no", E132="secondary"),-N132,0)</f>
+        <v>-1</v>
       </c>
       <c r="T132" s="0" t="n">
-        <f aca="false">IF(AND(R132="yes", E132="tertiary"),11-N132,0)</f>
+        <f aca="false">IF(AND(R132="yes", E132="secondary"),11-N132,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8765,11 +8765,11 @@
         <v>22</v>
       </c>
       <c r="S133" s="0" t="n">
-        <f aca="false">IF(AND(R133="no", E133="tertiary"),-N133,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R133="no", E133="secondary"),-N133,0)</f>
+        <v>-1</v>
       </c>
       <c r="T133" s="0" t="n">
-        <f aca="false">IF(AND(R133="yes", E133="tertiary"),11-N133,0)</f>
+        <f aca="false">IF(AND(R133="yes", E133="secondary"),11-N133,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8829,11 +8829,11 @@
         <v>22</v>
       </c>
       <c r="S134" s="0" t="n">
-        <f aca="false">IF(AND(R134="no", E134="tertiary"),-N134,0)</f>
+        <f aca="false">IF(AND(R134="no", E134="secondary"),-N134,0)</f>
         <v>0</v>
       </c>
       <c r="T134" s="0" t="n">
-        <f aca="false">IF(AND(R134="yes", E134="tertiary"),11-N134,0)</f>
+        <f aca="false">IF(AND(R134="yes", E134="secondary"),11-N134,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8893,11 +8893,11 @@
         <v>22</v>
       </c>
       <c r="S135" s="0" t="n">
-        <f aca="false">IF(AND(R135="no", E135="tertiary"),-N135,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R135="no", E135="secondary"),-N135,0)</f>
+        <v>-1</v>
       </c>
       <c r="T135" s="0" t="n">
-        <f aca="false">IF(AND(R135="yes", E135="tertiary"),11-N135,0)</f>
+        <f aca="false">IF(AND(R135="yes", E135="secondary"),11-N135,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8957,11 +8957,11 @@
         <v>22</v>
       </c>
       <c r="S136" s="0" t="n">
-        <f aca="false">IF(AND(R136="no", E136="tertiary"),-N136,0)</f>
+        <f aca="false">IF(AND(R136="no", E136="secondary"),-N136,0)</f>
         <v>0</v>
       </c>
       <c r="T136" s="0" t="n">
-        <f aca="false">IF(AND(R136="yes", E136="tertiary"),11-N136,0)</f>
+        <f aca="false">IF(AND(R136="yes", E136="secondary"),11-N136,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9021,11 +9021,11 @@
         <v>22</v>
       </c>
       <c r="S137" s="0" t="n">
-        <f aca="false">IF(AND(R137="no", E137="tertiary"),-N137,0)</f>
+        <f aca="false">IF(AND(R137="no", E137="secondary"),-N137,0)</f>
         <v>0</v>
       </c>
       <c r="T137" s="0" t="n">
-        <f aca="false">IF(AND(R137="yes", E137="tertiary"),11-N137,0)</f>
+        <f aca="false">IF(AND(R137="yes", E137="secondary"),11-N137,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9085,11 +9085,11 @@
         <v>22</v>
       </c>
       <c r="S138" s="0" t="n">
-        <f aca="false">IF(AND(R138="no", E138="tertiary"),-N138,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R138="no", E138="secondary"),-N138,0)</f>
+        <v>-2</v>
       </c>
       <c r="T138" s="0" t="n">
-        <f aca="false">IF(AND(R138="yes", E138="tertiary"),11-N138,0)</f>
+        <f aca="false">IF(AND(R138="yes", E138="secondary"),11-N138,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9149,11 +9149,11 @@
         <v>22</v>
       </c>
       <c r="S139" s="0" t="n">
-        <f aca="false">IF(AND(R139="no", E139="tertiary"),-N139,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R139="no", E139="secondary"),-N139,0)</f>
+        <v>0</v>
       </c>
       <c r="T139" s="0" t="n">
-        <f aca="false">IF(AND(R139="yes", E139="tertiary"),11-N139,0)</f>
+        <f aca="false">IF(AND(R139="yes", E139="secondary"),11-N139,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9213,11 +9213,11 @@
         <v>22</v>
       </c>
       <c r="S140" s="0" t="n">
-        <f aca="false">IF(AND(R140="no", E140="tertiary"),-N140,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R140="no", E140="secondary"),-N140,0)</f>
+        <v>-1</v>
       </c>
       <c r="T140" s="0" t="n">
-        <f aca="false">IF(AND(R140="yes", E140="tertiary"),11-N140,0)</f>
+        <f aca="false">IF(AND(R140="yes", E140="secondary"),11-N140,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9277,11 +9277,11 @@
         <v>22</v>
       </c>
       <c r="S141" s="0" t="n">
-        <f aca="false">IF(AND(R141="no", E141="tertiary"),-N141,0)</f>
+        <f aca="false">IF(AND(R141="no", E141="secondary"),-N141,0)</f>
         <v>0</v>
       </c>
       <c r="T141" s="0" t="n">
-        <f aca="false">IF(AND(R141="yes", E141="tertiary"),11-N141,0)</f>
+        <f aca="false">IF(AND(R141="yes", E141="secondary"),11-N141,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9341,11 +9341,11 @@
         <v>22</v>
       </c>
       <c r="S142" s="0" t="n">
-        <f aca="false">IF(AND(R142="no", E142="tertiary"),-N142,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R142="no", E142="secondary"),-N142,0)</f>
+        <v>-2</v>
       </c>
       <c r="T142" s="0" t="n">
-        <f aca="false">IF(AND(R142="yes", E142="tertiary"),11-N142,0)</f>
+        <f aca="false">IF(AND(R142="yes", E142="secondary"),11-N142,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9405,11 +9405,11 @@
         <v>22</v>
       </c>
       <c r="S143" s="0" t="n">
-        <f aca="false">IF(AND(R143="no", E143="tertiary"),-N143,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R143="no", E143="secondary"),-N143,0)</f>
+        <v>-1</v>
       </c>
       <c r="T143" s="0" t="n">
-        <f aca="false">IF(AND(R143="yes", E143="tertiary"),11-N143,0)</f>
+        <f aca="false">IF(AND(R143="yes", E143="secondary"),11-N143,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9469,11 +9469,11 @@
         <v>22</v>
       </c>
       <c r="S144" s="0" t="n">
-        <f aca="false">IF(AND(R144="no", E144="tertiary"),-N144,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R144="no", E144="secondary"),-N144,0)</f>
+        <v>-3</v>
       </c>
       <c r="T144" s="0" t="n">
-        <f aca="false">IF(AND(R144="yes", E144="tertiary"),11-N144,0)</f>
+        <f aca="false">IF(AND(R144="yes", E144="secondary"),11-N144,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9533,11 +9533,11 @@
         <v>22</v>
       </c>
       <c r="S145" s="0" t="n">
-        <f aca="false">IF(AND(R145="no", E145="tertiary"),-N145,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R145="no", E145="secondary"),-N145,0)</f>
+        <v>-2</v>
       </c>
       <c r="T145" s="0" t="n">
-        <f aca="false">IF(AND(R145="yes", E145="tertiary"),11-N145,0)</f>
+        <f aca="false">IF(AND(R145="yes", E145="secondary"),11-N145,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9597,11 +9597,11 @@
         <v>22</v>
       </c>
       <c r="S146" s="0" t="n">
-        <f aca="false">IF(AND(R146="no", E146="tertiary"),-N146,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R146="no", E146="secondary"),-N146,0)</f>
+        <v>0</v>
       </c>
       <c r="T146" s="0" t="n">
-        <f aca="false">IF(AND(R146="yes", E146="tertiary"),11-N146,0)</f>
+        <f aca="false">IF(AND(R146="yes", E146="secondary"),11-N146,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9661,11 +9661,11 @@
         <v>22</v>
       </c>
       <c r="S147" s="0" t="n">
-        <f aca="false">IF(AND(R147="no", E147="tertiary"),-N147,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R147="no", E147="secondary"),-N147,0)</f>
+        <v>-2</v>
       </c>
       <c r="T147" s="0" t="n">
-        <f aca="false">IF(AND(R147="yes", E147="tertiary"),11-N147,0)</f>
+        <f aca="false">IF(AND(R147="yes", E147="secondary"),11-N147,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9725,11 +9725,11 @@
         <v>22</v>
       </c>
       <c r="S148" s="0" t="n">
-        <f aca="false">IF(AND(R148="no", E148="tertiary"),-N148,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R148="no", E148="secondary"),-N148,0)</f>
+        <v>-5</v>
       </c>
       <c r="T148" s="0" t="n">
-        <f aca="false">IF(AND(R148="yes", E148="tertiary"),11-N148,0)</f>
+        <f aca="false">IF(AND(R148="yes", E148="secondary"),11-N148,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9789,11 +9789,11 @@
         <v>22</v>
       </c>
       <c r="S149" s="0" t="n">
-        <f aca="false">IF(AND(R149="no", E149="tertiary"),-N149,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R149="no", E149="secondary"),-N149,0)</f>
+        <v>-1</v>
       </c>
       <c r="T149" s="0" t="n">
-        <f aca="false">IF(AND(R149="yes", E149="tertiary"),11-N149,0)</f>
+        <f aca="false">IF(AND(R149="yes", E149="secondary"),11-N149,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9853,11 +9853,11 @@
         <v>22</v>
       </c>
       <c r="S150" s="0" t="n">
-        <f aca="false">IF(AND(R150="no", E150="tertiary"),-N150,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R150="no", E150="secondary"),-N150,0)</f>
+        <v>-1</v>
       </c>
       <c r="T150" s="0" t="n">
-        <f aca="false">IF(AND(R150="yes", E150="tertiary"),11-N150,0)</f>
+        <f aca="false">IF(AND(R150="yes", E150="secondary"),11-N150,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9917,11 +9917,11 @@
         <v>22</v>
       </c>
       <c r="S151" s="0" t="n">
-        <f aca="false">IF(AND(R151="no", E151="tertiary"),-N151,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R151="no", E151="secondary"),-N151,0)</f>
+        <v>0</v>
       </c>
       <c r="T151" s="0" t="n">
-        <f aca="false">IF(AND(R151="yes", E151="tertiary"),11-N151,0)</f>
+        <f aca="false">IF(AND(R151="yes", E151="secondary"),11-N151,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9981,11 +9981,11 @@
         <v>22</v>
       </c>
       <c r="S152" s="0" t="n">
-        <f aca="false">IF(AND(R152="no", E152="tertiary"),-N152,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R152="no", E152="secondary"),-N152,0)</f>
+        <v>-1</v>
       </c>
       <c r="T152" s="0" t="n">
-        <f aca="false">IF(AND(R152="yes", E152="tertiary"),11-N152,0)</f>
+        <f aca="false">IF(AND(R152="yes", E152="secondary"),11-N152,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10045,12 +10045,12 @@
         <v>23</v>
       </c>
       <c r="S153" s="0" t="n">
-        <f aca="false">IF(AND(R153="no", E153="tertiary"),-N153,0)</f>
+        <f aca="false">IF(AND(R153="no", E153="secondary"),-N153,0)</f>
         <v>0</v>
       </c>
       <c r="T153" s="0" t="n">
-        <f aca="false">IF(AND(R153="yes", E153="tertiary"),11-N153,0)</f>
-        <v>9</v>
+        <f aca="false">IF(AND(R153="yes", E153="secondary"),11-N153,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10109,11 +10109,11 @@
         <v>22</v>
       </c>
       <c r="S154" s="0" t="n">
-        <f aca="false">IF(AND(R154="no", E154="tertiary"),-N154,0)</f>
+        <f aca="false">IF(AND(R154="no", E154="secondary"),-N154,0)</f>
         <v>0</v>
       </c>
       <c r="T154" s="0" t="n">
-        <f aca="false">IF(AND(R154="yes", E154="tertiary"),11-N154,0)</f>
+        <f aca="false">IF(AND(R154="yes", E154="secondary"),11-N154,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10173,11 +10173,11 @@
         <v>22</v>
       </c>
       <c r="S155" s="0" t="n">
-        <f aca="false">IF(AND(R155="no", E155="tertiary"),-N155,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R155="no", E155="secondary"),-N155,0)</f>
+        <v>-1</v>
       </c>
       <c r="T155" s="0" t="n">
-        <f aca="false">IF(AND(R155="yes", E155="tertiary"),11-N155,0)</f>
+        <f aca="false">IF(AND(R155="yes", E155="secondary"),11-N155,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10237,11 +10237,11 @@
         <v>22</v>
       </c>
       <c r="S156" s="0" t="n">
-        <f aca="false">IF(AND(R156="no", E156="tertiary"),-N156,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R156="no", E156="secondary"),-N156,0)</f>
+        <v>-1</v>
       </c>
       <c r="T156" s="0" t="n">
-        <f aca="false">IF(AND(R156="yes", E156="tertiary"),11-N156,0)</f>
+        <f aca="false">IF(AND(R156="yes", E156="secondary"),11-N156,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10301,11 +10301,11 @@
         <v>22</v>
       </c>
       <c r="S157" s="0" t="n">
-        <f aca="false">IF(AND(R157="no", E157="tertiary"),-N157,0)</f>
+        <f aca="false">IF(AND(R157="no", E157="secondary"),-N157,0)</f>
         <v>0</v>
       </c>
       <c r="T157" s="0" t="n">
-        <f aca="false">IF(AND(R157="yes", E157="tertiary"),11-N157,0)</f>
+        <f aca="false">IF(AND(R157="yes", E157="secondary"),11-N157,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10365,11 +10365,11 @@
         <v>22</v>
       </c>
       <c r="S158" s="0" t="n">
-        <f aca="false">IF(AND(R158="no", E158="tertiary"),-N158,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R158="no", E158="secondary"),-N158,0)</f>
+        <v>-1</v>
       </c>
       <c r="T158" s="0" t="n">
-        <f aca="false">IF(AND(R158="yes", E158="tertiary"),11-N158,0)</f>
+        <f aca="false">IF(AND(R158="yes", E158="secondary"),11-N158,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10429,11 +10429,11 @@
         <v>22</v>
       </c>
       <c r="S159" s="0" t="n">
-        <f aca="false">IF(AND(R159="no", E159="tertiary"),-N159,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R159="no", E159="secondary"),-N159,0)</f>
+        <v>-1</v>
       </c>
       <c r="T159" s="0" t="n">
-        <f aca="false">IF(AND(R159="yes", E159="tertiary"),11-N159,0)</f>
+        <f aca="false">IF(AND(R159="yes", E159="secondary"),11-N159,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10493,11 +10493,11 @@
         <v>22</v>
       </c>
       <c r="S160" s="0" t="n">
-        <f aca="false">IF(AND(R160="no", E160="tertiary"),-N160,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R160="no", E160="secondary"),-N160,0)</f>
+        <v>-2</v>
       </c>
       <c r="T160" s="0" t="n">
-        <f aca="false">IF(AND(R160="yes", E160="tertiary"),11-N160,0)</f>
+        <f aca="false">IF(AND(R160="yes", E160="secondary"),11-N160,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10557,11 +10557,11 @@
         <v>22</v>
       </c>
       <c r="S161" s="0" t="n">
-        <f aca="false">IF(AND(R161="no", E161="tertiary"),-N161,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R161="no", E161="secondary"),-N161,0)</f>
+        <v>-2</v>
       </c>
       <c r="T161" s="0" t="n">
-        <f aca="false">IF(AND(R161="yes", E161="tertiary"),11-N161,0)</f>
+        <f aca="false">IF(AND(R161="yes", E161="secondary"),11-N161,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10621,11 +10621,11 @@
         <v>22</v>
       </c>
       <c r="S162" s="0" t="n">
-        <f aca="false">IF(AND(R162="no", E162="tertiary"),-N162,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R162="no", E162="secondary"),-N162,0)</f>
+        <v>-2</v>
       </c>
       <c r="T162" s="0" t="n">
-        <f aca="false">IF(AND(R162="yes", E162="tertiary"),11-N162,0)</f>
+        <f aca="false">IF(AND(R162="yes", E162="secondary"),11-N162,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10685,11 +10685,11 @@
         <v>22</v>
       </c>
       <c r="S163" s="0" t="n">
-        <f aca="false">IF(AND(R163="no", E163="tertiary"),-N163,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R163="no", E163="secondary"),-N163,0)</f>
+        <v>-1</v>
       </c>
       <c r="T163" s="0" t="n">
-        <f aca="false">IF(AND(R163="yes", E163="tertiary"),11-N163,0)</f>
+        <f aca="false">IF(AND(R163="yes", E163="secondary"),11-N163,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10749,11 +10749,11 @@
         <v>22</v>
       </c>
       <c r="S164" s="0" t="n">
-        <f aca="false">IF(AND(R164="no", E164="tertiary"),-N164,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R164="no", E164="secondary"),-N164,0)</f>
+        <v>0</v>
       </c>
       <c r="T164" s="0" t="n">
-        <f aca="false">IF(AND(R164="yes", E164="tertiary"),11-N164,0)</f>
+        <f aca="false">IF(AND(R164="yes", E164="secondary"),11-N164,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10813,11 +10813,11 @@
         <v>22</v>
       </c>
       <c r="S165" s="0" t="n">
-        <f aca="false">IF(AND(R165="no", E165="tertiary"),-N165,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R165="no", E165="secondary"),-N165,0)</f>
+        <v>-2</v>
       </c>
       <c r="T165" s="0" t="n">
-        <f aca="false">IF(AND(R165="yes", E165="tertiary"),11-N165,0)</f>
+        <f aca="false">IF(AND(R165="yes", E165="secondary"),11-N165,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10877,11 +10877,11 @@
         <v>22</v>
       </c>
       <c r="S166" s="0" t="n">
-        <f aca="false">IF(AND(R166="no", E166="tertiary"),-N166,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R166="no", E166="secondary"),-N166,0)</f>
+        <v>-1</v>
       </c>
       <c r="T166" s="0" t="n">
-        <f aca="false">IF(AND(R166="yes", E166="tertiary"),11-N166,0)</f>
+        <f aca="false">IF(AND(R166="yes", E166="secondary"),11-N166,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10941,11 +10941,11 @@
         <v>22</v>
       </c>
       <c r="S167" s="0" t="n">
-        <f aca="false">IF(AND(R167="no", E167="tertiary"),-N167,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R167="no", E167="secondary"),-N167,0)</f>
+        <v>-1</v>
       </c>
       <c r="T167" s="0" t="n">
-        <f aca="false">IF(AND(R167="yes", E167="tertiary"),11-N167,0)</f>
+        <f aca="false">IF(AND(R167="yes", E167="secondary"),11-N167,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11005,11 +11005,11 @@
         <v>22</v>
       </c>
       <c r="S168" s="0" t="n">
-        <f aca="false">IF(AND(R168="no", E168="tertiary"),-N168,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R168="no", E168="secondary"),-N168,0)</f>
+        <v>0</v>
       </c>
       <c r="T168" s="0" t="n">
-        <f aca="false">IF(AND(R168="yes", E168="tertiary"),11-N168,0)</f>
+        <f aca="false">IF(AND(R168="yes", E168="secondary"),11-N168,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11069,11 +11069,11 @@
         <v>22</v>
       </c>
       <c r="S169" s="0" t="n">
-        <f aca="false">IF(AND(R169="no", E169="tertiary"),-N169,0)</f>
+        <f aca="false">IF(AND(R169="no", E169="secondary"),-N169,0)</f>
         <v>0</v>
       </c>
       <c r="T169" s="0" t="n">
-        <f aca="false">IF(AND(R169="yes", E169="tertiary"),11-N169,0)</f>
+        <f aca="false">IF(AND(R169="yes", E169="secondary"),11-N169,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11133,11 +11133,11 @@
         <v>22</v>
       </c>
       <c r="S170" s="0" t="n">
-        <f aca="false">IF(AND(R170="no", E170="tertiary"),-N170,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R170="no", E170="secondary"),-N170,0)</f>
+        <v>-1</v>
       </c>
       <c r="T170" s="0" t="n">
-        <f aca="false">IF(AND(R170="yes", E170="tertiary"),11-N170,0)</f>
+        <f aca="false">IF(AND(R170="yes", E170="secondary"),11-N170,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11197,11 +11197,11 @@
         <v>22</v>
       </c>
       <c r="S171" s="0" t="n">
-        <f aca="false">IF(AND(R171="no", E171="tertiary"),-N171,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R171="no", E171="secondary"),-N171,0)</f>
+        <v>-1</v>
       </c>
       <c r="T171" s="0" t="n">
-        <f aca="false">IF(AND(R171="yes", E171="tertiary"),11-N171,0)</f>
+        <f aca="false">IF(AND(R171="yes", E171="secondary"),11-N171,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11261,11 +11261,11 @@
         <v>22</v>
       </c>
       <c r="S172" s="0" t="n">
-        <f aca="false">IF(AND(R172="no", E172="tertiary"),-N172,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R172="no", E172="secondary"),-N172,0)</f>
+        <v>0</v>
       </c>
       <c r="T172" s="0" t="n">
-        <f aca="false">IF(AND(R172="yes", E172="tertiary"),11-N172,0)</f>
+        <f aca="false">IF(AND(R172="yes", E172="secondary"),11-N172,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11325,11 +11325,11 @@
         <v>22</v>
       </c>
       <c r="S173" s="0" t="n">
-        <f aca="false">IF(AND(R173="no", E173="tertiary"),-N173,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R173="no", E173="secondary"),-N173,0)</f>
+        <v>-1</v>
       </c>
       <c r="T173" s="0" t="n">
-        <f aca="false">IF(AND(R173="yes", E173="tertiary"),11-N173,0)</f>
+        <f aca="false">IF(AND(R173="yes", E173="secondary"),11-N173,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11389,11 +11389,11 @@
         <v>22</v>
       </c>
       <c r="S174" s="0" t="n">
-        <f aca="false">IF(AND(R174="no", E174="tertiary"),-N174,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R174="no", E174="secondary"),-N174,0)</f>
+        <v>0</v>
       </c>
       <c r="T174" s="0" t="n">
-        <f aca="false">IF(AND(R174="yes", E174="tertiary"),11-N174,0)</f>
+        <f aca="false">IF(AND(R174="yes", E174="secondary"),11-N174,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11453,11 +11453,11 @@
         <v>22</v>
       </c>
       <c r="S175" s="0" t="n">
-        <f aca="false">IF(AND(R175="no", E175="tertiary"),-N175,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R175="no", E175="secondary"),-N175,0)</f>
+        <v>0</v>
       </c>
       <c r="T175" s="0" t="n">
-        <f aca="false">IF(AND(R175="yes", E175="tertiary"),11-N175,0)</f>
+        <f aca="false">IF(AND(R175="yes", E175="secondary"),11-N175,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11517,11 +11517,11 @@
         <v>22</v>
       </c>
       <c r="S176" s="0" t="n">
-        <f aca="false">IF(AND(R176="no", E176="tertiary"),-N176,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R176="no", E176="secondary"),-N176,0)</f>
+        <v>-1</v>
       </c>
       <c r="T176" s="0" t="n">
-        <f aca="false">IF(AND(R176="yes", E176="tertiary"),11-N176,0)</f>
+        <f aca="false">IF(AND(R176="yes", E176="secondary"),11-N176,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11581,11 +11581,11 @@
         <v>22</v>
       </c>
       <c r="S177" s="0" t="n">
-        <f aca="false">IF(AND(R177="no", E177="tertiary"),-N177,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R177="no", E177="secondary"),-N177,0)</f>
+        <v>-1</v>
       </c>
       <c r="T177" s="0" t="n">
-        <f aca="false">IF(AND(R177="yes", E177="tertiary"),11-N177,0)</f>
+        <f aca="false">IF(AND(R177="yes", E177="secondary"),11-N177,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11645,11 +11645,11 @@
         <v>22</v>
       </c>
       <c r="S178" s="0" t="n">
-        <f aca="false">IF(AND(R178="no", E178="tertiary"),-N178,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R178="no", E178="secondary"),-N178,0)</f>
+        <v>-2</v>
       </c>
       <c r="T178" s="0" t="n">
-        <f aca="false">IF(AND(R178="yes", E178="tertiary"),11-N178,0)</f>
+        <f aca="false">IF(AND(R178="yes", E178="secondary"),11-N178,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11709,11 +11709,11 @@
         <v>22</v>
       </c>
       <c r="S179" s="0" t="n">
-        <f aca="false">IF(AND(R179="no", E179="tertiary"),-N179,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R179="no", E179="secondary"),-N179,0)</f>
+        <v>-1</v>
       </c>
       <c r="T179" s="0" t="n">
-        <f aca="false">IF(AND(R179="yes", E179="tertiary"),11-N179,0)</f>
+        <f aca="false">IF(AND(R179="yes", E179="secondary"),11-N179,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11773,11 +11773,11 @@
         <v>22</v>
       </c>
       <c r="S180" s="0" t="n">
-        <f aca="false">IF(AND(R180="no", E180="tertiary"),-N180,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R180="no", E180="secondary"),-N180,0)</f>
+        <v>0</v>
       </c>
       <c r="T180" s="0" t="n">
-        <f aca="false">IF(AND(R180="yes", E180="tertiary"),11-N180,0)</f>
+        <f aca="false">IF(AND(R180="yes", E180="secondary"),11-N180,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11837,11 +11837,11 @@
         <v>22</v>
       </c>
       <c r="S181" s="0" t="n">
-        <f aca="false">IF(AND(R181="no", E181="tertiary"),-N181,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R181="no", E181="secondary"),-N181,0)</f>
+        <v>0</v>
       </c>
       <c r="T181" s="0" t="n">
-        <f aca="false">IF(AND(R181="yes", E181="tertiary"),11-N181,0)</f>
+        <f aca="false">IF(AND(R181="yes", E181="secondary"),11-N181,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11901,11 +11901,11 @@
         <v>22</v>
       </c>
       <c r="S182" s="0" t="n">
-        <f aca="false">IF(AND(R182="no", E182="tertiary"),-N182,0)</f>
+        <f aca="false">IF(AND(R182="no", E182="secondary"),-N182,0)</f>
         <v>0</v>
       </c>
       <c r="T182" s="0" t="n">
-        <f aca="false">IF(AND(R182="yes", E182="tertiary"),11-N182,0)</f>
+        <f aca="false">IF(AND(R182="yes", E182="secondary"),11-N182,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11965,11 +11965,11 @@
         <v>22</v>
       </c>
       <c r="S183" s="0" t="n">
-        <f aca="false">IF(AND(R183="no", E183="tertiary"),-N183,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R183="no", E183="secondary"),-N183,0)</f>
+        <v>-1</v>
       </c>
       <c r="T183" s="0" t="n">
-        <f aca="false">IF(AND(R183="yes", E183="tertiary"),11-N183,0)</f>
+        <f aca="false">IF(AND(R183="yes", E183="secondary"),11-N183,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12029,11 +12029,11 @@
         <v>22</v>
       </c>
       <c r="S184" s="0" t="n">
-        <f aca="false">IF(AND(R184="no", E184="tertiary"),-N184,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R184="no", E184="secondary"),-N184,0)</f>
+        <v>0</v>
       </c>
       <c r="T184" s="0" t="n">
-        <f aca="false">IF(AND(R184="yes", E184="tertiary"),11-N184,0)</f>
+        <f aca="false">IF(AND(R184="yes", E184="secondary"),11-N184,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12093,11 +12093,11 @@
         <v>22</v>
       </c>
       <c r="S185" s="0" t="n">
-        <f aca="false">IF(AND(R185="no", E185="tertiary"),-N185,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R185="no", E185="secondary"),-N185,0)</f>
+        <v>-1</v>
       </c>
       <c r="T185" s="0" t="n">
-        <f aca="false">IF(AND(R185="yes", E185="tertiary"),11-N185,0)</f>
+        <f aca="false">IF(AND(R185="yes", E185="secondary"),11-N185,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12157,11 +12157,11 @@
         <v>22</v>
       </c>
       <c r="S186" s="0" t="n">
-        <f aca="false">IF(AND(R186="no", E186="tertiary"),-N186,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R186="no", E186="secondary"),-N186,0)</f>
+        <v>-1</v>
       </c>
       <c r="T186" s="0" t="n">
-        <f aca="false">IF(AND(R186="yes", E186="tertiary"),11-N186,0)</f>
+        <f aca="false">IF(AND(R186="yes", E186="secondary"),11-N186,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12221,11 +12221,11 @@
         <v>22</v>
       </c>
       <c r="S187" s="0" t="n">
-        <f aca="false">IF(AND(R187="no", E187="tertiary"),-N187,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R187="no", E187="secondary"),-N187,0)</f>
+        <v>-2</v>
       </c>
       <c r="T187" s="0" t="n">
-        <f aca="false">IF(AND(R187="yes", E187="tertiary"),11-N187,0)</f>
+        <f aca="false">IF(AND(R187="yes", E187="secondary"),11-N187,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12285,11 +12285,11 @@
         <v>22</v>
       </c>
       <c r="S188" s="0" t="n">
-        <f aca="false">IF(AND(R188="no", E188="tertiary"),-N188,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R188="no", E188="secondary"),-N188,0)</f>
+        <v>0</v>
       </c>
       <c r="T188" s="0" t="n">
-        <f aca="false">IF(AND(R188="yes", E188="tertiary"),11-N188,0)</f>
+        <f aca="false">IF(AND(R188="yes", E188="secondary"),11-N188,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12349,11 +12349,11 @@
         <v>22</v>
       </c>
       <c r="S189" s="0" t="n">
-        <f aca="false">IF(AND(R189="no", E189="tertiary"),-N189,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R189="no", E189="secondary"),-N189,0)</f>
+        <v>0</v>
       </c>
       <c r="T189" s="0" t="n">
-        <f aca="false">IF(AND(R189="yes", E189="tertiary"),11-N189,0)</f>
+        <f aca="false">IF(AND(R189="yes", E189="secondary"),11-N189,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12413,11 +12413,11 @@
         <v>22</v>
       </c>
       <c r="S190" s="0" t="n">
-        <f aca="false">IF(AND(R190="no", E190="tertiary"),-N190,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R190="no", E190="secondary"),-N190,0)</f>
+        <v>-1</v>
       </c>
       <c r="T190" s="0" t="n">
-        <f aca="false">IF(AND(R190="yes", E190="tertiary"),11-N190,0)</f>
+        <f aca="false">IF(AND(R190="yes", E190="secondary"),11-N190,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12477,11 +12477,11 @@
         <v>22</v>
       </c>
       <c r="S191" s="0" t="n">
-        <f aca="false">IF(AND(R191="no", E191="tertiary"),-N191,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R191="no", E191="secondary"),-N191,0)</f>
+        <v>-1</v>
       </c>
       <c r="T191" s="0" t="n">
-        <f aca="false">IF(AND(R191="yes", E191="tertiary"),11-N191,0)</f>
+        <f aca="false">IF(AND(R191="yes", E191="secondary"),11-N191,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12541,11 +12541,11 @@
         <v>22</v>
       </c>
       <c r="S192" s="0" t="n">
-        <f aca="false">IF(AND(R192="no", E192="tertiary"),-N192,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R192="no", E192="secondary"),-N192,0)</f>
+        <v>-2</v>
       </c>
       <c r="T192" s="0" t="n">
-        <f aca="false">IF(AND(R192="yes", E192="tertiary"),11-N192,0)</f>
+        <f aca="false">IF(AND(R192="yes", E192="secondary"),11-N192,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12605,11 +12605,11 @@
         <v>22</v>
       </c>
       <c r="S193" s="0" t="n">
-        <f aca="false">IF(AND(R193="no", E193="tertiary"),-N193,0)</f>
+        <f aca="false">IF(AND(R193="no", E193="secondary"),-N193,0)</f>
         <v>0</v>
       </c>
       <c r="T193" s="0" t="n">
-        <f aca="false">IF(AND(R193="yes", E193="tertiary"),11-N193,0)</f>
+        <f aca="false">IF(AND(R193="yes", E193="secondary"),11-N193,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12669,11 +12669,11 @@
         <v>22</v>
       </c>
       <c r="S194" s="0" t="n">
-        <f aca="false">IF(AND(R194="no", E194="tertiary"),-N194,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R194="no", E194="secondary"),-N194,0)</f>
+        <v>-1</v>
       </c>
       <c r="T194" s="0" t="n">
-        <f aca="false">IF(AND(R194="yes", E194="tertiary"),11-N194,0)</f>
+        <f aca="false">IF(AND(R194="yes", E194="secondary"),11-N194,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12733,11 +12733,11 @@
         <v>22</v>
       </c>
       <c r="S195" s="0" t="n">
-        <f aca="false">IF(AND(R195="no", E195="tertiary"),-N195,0)</f>
+        <f aca="false">IF(AND(R195="no", E195="secondary"),-N195,0)</f>
         <v>0</v>
       </c>
       <c r="T195" s="0" t="n">
-        <f aca="false">IF(AND(R195="yes", E195="tertiary"),11-N195,0)</f>
+        <f aca="false">IF(AND(R195="yes", E195="secondary"),11-N195,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12797,11 +12797,11 @@
         <v>22</v>
       </c>
       <c r="S196" s="0" t="n">
-        <f aca="false">IF(AND(R196="no", E196="tertiary"),-N196,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R196="no", E196="secondary"),-N196,0)</f>
+        <v>0</v>
       </c>
       <c r="T196" s="0" t="n">
-        <f aca="false">IF(AND(R196="yes", E196="tertiary"),11-N196,0)</f>
+        <f aca="false">IF(AND(R196="yes", E196="secondary"),11-N196,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12861,11 +12861,11 @@
         <v>22</v>
       </c>
       <c r="S197" s="0" t="n">
-        <f aca="false">IF(AND(R197="no", E197="tertiary"),-N197,0)</f>
+        <f aca="false">IF(AND(R197="no", E197="secondary"),-N197,0)</f>
         <v>0</v>
       </c>
       <c r="T197" s="0" t="n">
-        <f aca="false">IF(AND(R197="yes", E197="tertiary"),11-N197,0)</f>
+        <f aca="false">IF(AND(R197="yes", E197="secondary"),11-N197,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12925,11 +12925,11 @@
         <v>22</v>
       </c>
       <c r="S198" s="0" t="n">
-        <f aca="false">IF(AND(R198="no", E198="tertiary"),-N198,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R198="no", E198="secondary"),-N198,0)</f>
+        <v>0</v>
       </c>
       <c r="T198" s="0" t="n">
-        <f aca="false">IF(AND(R198="yes", E198="tertiary"),11-N198,0)</f>
+        <f aca="false">IF(AND(R198="yes", E198="secondary"),11-N198,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12989,11 +12989,11 @@
         <v>22</v>
       </c>
       <c r="S199" s="0" t="n">
-        <f aca="false">IF(AND(R199="no", E199="tertiary"),-N199,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R199="no", E199="secondary"),-N199,0)</f>
+        <v>-1</v>
       </c>
       <c r="T199" s="0" t="n">
-        <f aca="false">IF(AND(R199="yes", E199="tertiary"),11-N199,0)</f>
+        <f aca="false">IF(AND(R199="yes", E199="secondary"),11-N199,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13053,11 +13053,11 @@
         <v>22</v>
       </c>
       <c r="S200" s="0" t="n">
-        <f aca="false">IF(AND(R200="no", E200="tertiary"),-N200,0)</f>
+        <f aca="false">IF(AND(R200="no", E200="secondary"),-N200,0)</f>
         <v>0</v>
       </c>
       <c r="T200" s="0" t="n">
-        <f aca="false">IF(AND(R200="yes", E200="tertiary"),11-N200,0)</f>
+        <f aca="false">IF(AND(R200="yes", E200="secondary"),11-N200,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13117,11 +13117,11 @@
         <v>22</v>
       </c>
       <c r="S201" s="0" t="n">
-        <f aca="false">IF(AND(R201="no", E201="tertiary"),-N201,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R201="no", E201="secondary"),-N201,0)</f>
+        <v>-1</v>
       </c>
       <c r="T201" s="0" t="n">
-        <f aca="false">IF(AND(R201="yes", E201="tertiary"),11-N201,0)</f>
+        <f aca="false">IF(AND(R201="yes", E201="secondary"),11-N201,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13181,11 +13181,11 @@
         <v>22</v>
       </c>
       <c r="S202" s="0" t="n">
-        <f aca="false">IF(AND(R202="no", E202="tertiary"),-N202,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R202="no", E202="secondary"),-N202,0)</f>
+        <v>-1</v>
       </c>
       <c r="T202" s="0" t="n">
-        <f aca="false">IF(AND(R202="yes", E202="tertiary"),11-N202,0)</f>
+        <f aca="false">IF(AND(R202="yes", E202="secondary"),11-N202,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13245,11 +13245,11 @@
         <v>22</v>
       </c>
       <c r="S203" s="0" t="n">
-        <f aca="false">IF(AND(R203="no", E203="tertiary"),-N203,0)</f>
+        <f aca="false">IF(AND(R203="no", E203="secondary"),-N203,0)</f>
         <v>0</v>
       </c>
       <c r="T203" s="0" t="n">
-        <f aca="false">IF(AND(R203="yes", E203="tertiary"),11-N203,0)</f>
+        <f aca="false">IF(AND(R203="yes", E203="secondary"),11-N203,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13309,11 +13309,11 @@
         <v>22</v>
       </c>
       <c r="S204" s="0" t="n">
-        <f aca="false">IF(AND(R204="no", E204="tertiary"),-N204,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R204="no", E204="secondary"),-N204,0)</f>
+        <v>0</v>
       </c>
       <c r="T204" s="0" t="n">
-        <f aca="false">IF(AND(R204="yes", E204="tertiary"),11-N204,0)</f>
+        <f aca="false">IF(AND(R204="yes", E204="secondary"),11-N204,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13373,11 +13373,11 @@
         <v>22</v>
       </c>
       <c r="S205" s="0" t="n">
-        <f aca="false">IF(AND(R205="no", E205="tertiary"),-N205,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R205="no", E205="secondary"),-N205,0)</f>
+        <v>-1</v>
       </c>
       <c r="T205" s="0" t="n">
-        <f aca="false">IF(AND(R205="yes", E205="tertiary"),11-N205,0)</f>
+        <f aca="false">IF(AND(R205="yes", E205="secondary"),11-N205,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13437,11 +13437,11 @@
         <v>22</v>
       </c>
       <c r="S206" s="0" t="n">
-        <f aca="false">IF(AND(R206="no", E206="tertiary"),-N206,0)</f>
+        <f aca="false">IF(AND(R206="no", E206="secondary"),-N206,0)</f>
         <v>0</v>
       </c>
       <c r="T206" s="0" t="n">
-        <f aca="false">IF(AND(R206="yes", E206="tertiary"),11-N206,0)</f>
+        <f aca="false">IF(AND(R206="yes", E206="secondary"),11-N206,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13501,11 +13501,11 @@
         <v>22</v>
       </c>
       <c r="S207" s="0" t="n">
-        <f aca="false">IF(AND(R207="no", E207="tertiary"),-N207,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R207="no", E207="secondary"),-N207,0)</f>
+        <v>-2</v>
       </c>
       <c r="T207" s="0" t="n">
-        <f aca="false">IF(AND(R207="yes", E207="tertiary"),11-N207,0)</f>
+        <f aca="false">IF(AND(R207="yes", E207="secondary"),11-N207,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13565,11 +13565,11 @@
         <v>22</v>
       </c>
       <c r="S208" s="0" t="n">
-        <f aca="false">IF(AND(R208="no", E208="tertiary"),-N208,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R208="no", E208="secondary"),-N208,0)</f>
+        <v>-2</v>
       </c>
       <c r="T208" s="0" t="n">
-        <f aca="false">IF(AND(R208="yes", E208="tertiary"),11-N208,0)</f>
+        <f aca="false">IF(AND(R208="yes", E208="secondary"),11-N208,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13629,11 +13629,11 @@
         <v>22</v>
       </c>
       <c r="S209" s="0" t="n">
-        <f aca="false">IF(AND(R209="no", E209="tertiary"),-N209,0)</f>
+        <f aca="false">IF(AND(R209="no", E209="secondary"),-N209,0)</f>
         <v>0</v>
       </c>
       <c r="T209" s="0" t="n">
-        <f aca="false">IF(AND(R209="yes", E209="tertiary"),11-N209,0)</f>
+        <f aca="false">IF(AND(R209="yes", E209="secondary"),11-N209,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13693,11 +13693,11 @@
         <v>22</v>
       </c>
       <c r="S210" s="0" t="n">
-        <f aca="false">IF(AND(R210="no", E210="tertiary"),-N210,0)</f>
+        <f aca="false">IF(AND(R210="no", E210="secondary"),-N210,0)</f>
         <v>0</v>
       </c>
       <c r="T210" s="0" t="n">
-        <f aca="false">IF(AND(R210="yes", E210="tertiary"),11-N210,0)</f>
+        <f aca="false">IF(AND(R210="yes", E210="secondary"),11-N210,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13757,11 +13757,11 @@
         <v>22</v>
       </c>
       <c r="S211" s="0" t="n">
-        <f aca="false">IF(AND(R211="no", E211="tertiary"),-N211,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R211="no", E211="secondary"),-N211,0)</f>
+        <v>-2</v>
       </c>
       <c r="T211" s="0" t="n">
-        <f aca="false">IF(AND(R211="yes", E211="tertiary"),11-N211,0)</f>
+        <f aca="false">IF(AND(R211="yes", E211="secondary"),11-N211,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13821,11 +13821,11 @@
         <v>22</v>
       </c>
       <c r="S212" s="0" t="n">
-        <f aca="false">IF(AND(R212="no", E212="tertiary"),-N212,0)</f>
+        <f aca="false">IF(AND(R212="no", E212="secondary"),-N212,0)</f>
         <v>0</v>
       </c>
       <c r="T212" s="0" t="n">
-        <f aca="false">IF(AND(R212="yes", E212="tertiary"),11-N212,0)</f>
+        <f aca="false">IF(AND(R212="yes", E212="secondary"),11-N212,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13885,11 +13885,11 @@
         <v>22</v>
       </c>
       <c r="S213" s="0" t="n">
-        <f aca="false">IF(AND(R213="no", E213="tertiary"),-N213,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R213="no", E213="secondary"),-N213,0)</f>
+        <v>-1</v>
       </c>
       <c r="T213" s="0" t="n">
-        <f aca="false">IF(AND(R213="yes", E213="tertiary"),11-N213,0)</f>
+        <f aca="false">IF(AND(R213="yes", E213="secondary"),11-N213,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13949,11 +13949,11 @@
         <v>22</v>
       </c>
       <c r="S214" s="0" t="n">
-        <f aca="false">IF(AND(R214="no", E214="tertiary"),-N214,0)</f>
+        <f aca="false">IF(AND(R214="no", E214="secondary"),-N214,0)</f>
         <v>0</v>
       </c>
       <c r="T214" s="0" t="n">
-        <f aca="false">IF(AND(R214="yes", E214="tertiary"),11-N214,0)</f>
+        <f aca="false">IF(AND(R214="yes", E214="secondary"),11-N214,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14013,11 +14013,11 @@
         <v>22</v>
       </c>
       <c r="S215" s="0" t="n">
-        <f aca="false">IF(AND(R215="no", E215="tertiary"),-N215,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R215="no", E215="secondary"),-N215,0)</f>
+        <v>-1</v>
       </c>
       <c r="T215" s="0" t="n">
-        <f aca="false">IF(AND(R215="yes", E215="tertiary"),11-N215,0)</f>
+        <f aca="false">IF(AND(R215="yes", E215="secondary"),11-N215,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14077,11 +14077,11 @@
         <v>22</v>
       </c>
       <c r="S216" s="0" t="n">
-        <f aca="false">IF(AND(R216="no", E216="tertiary"),-N216,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R216="no", E216="secondary"),-N216,0)</f>
+        <v>-1</v>
       </c>
       <c r="T216" s="0" t="n">
-        <f aca="false">IF(AND(R216="yes", E216="tertiary"),11-N216,0)</f>
+        <f aca="false">IF(AND(R216="yes", E216="secondary"),11-N216,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14141,11 +14141,11 @@
         <v>22</v>
       </c>
       <c r="S217" s="0" t="n">
-        <f aca="false">IF(AND(R217="no", E217="tertiary"),-N217,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R217="no", E217="secondary"),-N217,0)</f>
+        <v>-1</v>
       </c>
       <c r="T217" s="0" t="n">
-        <f aca="false">IF(AND(R217="yes", E217="tertiary"),11-N217,0)</f>
+        <f aca="false">IF(AND(R217="yes", E217="secondary"),11-N217,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14205,11 +14205,11 @@
         <v>22</v>
       </c>
       <c r="S218" s="0" t="n">
-        <f aca="false">IF(AND(R218="no", E218="tertiary"),-N218,0)</f>
-        <v>-3</v>
+        <f aca="false">IF(AND(R218="no", E218="secondary"),-N218,0)</f>
+        <v>0</v>
       </c>
       <c r="T218" s="0" t="n">
-        <f aca="false">IF(AND(R218="yes", E218="tertiary"),11-N218,0)</f>
+        <f aca="false">IF(AND(R218="yes", E218="secondary"),11-N218,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14269,11 +14269,11 @@
         <v>22</v>
       </c>
       <c r="S219" s="0" t="n">
-        <f aca="false">IF(AND(R219="no", E219="tertiary"),-N219,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R219="no", E219="secondary"),-N219,0)</f>
+        <v>-2</v>
       </c>
       <c r="T219" s="0" t="n">
-        <f aca="false">IF(AND(R219="yes", E219="tertiary"),11-N219,0)</f>
+        <f aca="false">IF(AND(R219="yes", E219="secondary"),11-N219,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14333,11 +14333,11 @@
         <v>22</v>
       </c>
       <c r="S220" s="0" t="n">
-        <f aca="false">IF(AND(R220="no", E220="tertiary"),-N220,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R220="no", E220="secondary"),-N220,0)</f>
+        <v>0</v>
       </c>
       <c r="T220" s="0" t="n">
-        <f aca="false">IF(AND(R220="yes", E220="tertiary"),11-N220,0)</f>
+        <f aca="false">IF(AND(R220="yes", E220="secondary"),11-N220,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14397,11 +14397,11 @@
         <v>22</v>
       </c>
       <c r="S221" s="0" t="n">
-        <f aca="false">IF(AND(R221="no", E221="tertiary"),-N221,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R221="no", E221="secondary"),-N221,0)</f>
+        <v>-1</v>
       </c>
       <c r="T221" s="0" t="n">
-        <f aca="false">IF(AND(R221="yes", E221="tertiary"),11-N221,0)</f>
+        <f aca="false">IF(AND(R221="yes", E221="secondary"),11-N221,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14461,11 +14461,11 @@
         <v>22</v>
       </c>
       <c r="S222" s="0" t="n">
-        <f aca="false">IF(AND(R222="no", E222="tertiary"),-N222,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R222="no", E222="secondary"),-N222,0)</f>
+        <v>-2</v>
       </c>
       <c r="T222" s="0" t="n">
-        <f aca="false">IF(AND(R222="yes", E222="tertiary"),11-N222,0)</f>
+        <f aca="false">IF(AND(R222="yes", E222="secondary"),11-N222,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14525,11 +14525,11 @@
         <v>22</v>
       </c>
       <c r="S223" s="0" t="n">
-        <f aca="false">IF(AND(R223="no", E223="tertiary"),-N223,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R223="no", E223="secondary"),-N223,0)</f>
+        <v>-1</v>
       </c>
       <c r="T223" s="0" t="n">
-        <f aca="false">IF(AND(R223="yes", E223="tertiary"),11-N223,0)</f>
+        <f aca="false">IF(AND(R223="yes", E223="secondary"),11-N223,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14589,11 +14589,11 @@
         <v>22</v>
       </c>
       <c r="S224" s="0" t="n">
-        <f aca="false">IF(AND(R224="no", E224="tertiary"),-N224,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R224="no", E224="secondary"),-N224,0)</f>
+        <v>-1</v>
       </c>
       <c r="T224" s="0" t="n">
-        <f aca="false">IF(AND(R224="yes", E224="tertiary"),11-N224,0)</f>
+        <f aca="false">IF(AND(R224="yes", E224="secondary"),11-N224,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14653,11 +14653,11 @@
         <v>22</v>
       </c>
       <c r="S225" s="0" t="n">
-        <f aca="false">IF(AND(R225="no", E225="tertiary"),-N225,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R225="no", E225="secondary"),-N225,0)</f>
+        <v>-1</v>
       </c>
       <c r="T225" s="0" t="n">
-        <f aca="false">IF(AND(R225="yes", E225="tertiary"),11-N225,0)</f>
+        <f aca="false">IF(AND(R225="yes", E225="secondary"),11-N225,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14717,11 +14717,11 @@
         <v>22</v>
       </c>
       <c r="S226" s="0" t="n">
-        <f aca="false">IF(AND(R226="no", E226="tertiary"),-N226,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R226="no", E226="secondary"),-N226,0)</f>
+        <v>-1</v>
       </c>
       <c r="T226" s="0" t="n">
-        <f aca="false">IF(AND(R226="yes", E226="tertiary"),11-N226,0)</f>
+        <f aca="false">IF(AND(R226="yes", E226="secondary"),11-N226,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14781,11 +14781,11 @@
         <v>22</v>
       </c>
       <c r="S227" s="0" t="n">
-        <f aca="false">IF(AND(R227="no", E227="tertiary"),-N227,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R227="no", E227="secondary"),-N227,0)</f>
+        <v>0</v>
       </c>
       <c r="T227" s="0" t="n">
-        <f aca="false">IF(AND(R227="yes", E227="tertiary"),11-N227,0)</f>
+        <f aca="false">IF(AND(R227="yes", E227="secondary"),11-N227,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14845,11 +14845,11 @@
         <v>22</v>
       </c>
       <c r="S228" s="0" t="n">
-        <f aca="false">IF(AND(R228="no", E228="tertiary"),-N228,0)</f>
+        <f aca="false">IF(AND(R228="no", E228="secondary"),-N228,0)</f>
         <v>0</v>
       </c>
       <c r="T228" s="0" t="n">
-        <f aca="false">IF(AND(R228="yes", E228="tertiary"),11-N228,0)</f>
+        <f aca="false">IF(AND(R228="yes", E228="secondary"),11-N228,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14909,11 +14909,11 @@
         <v>22</v>
       </c>
       <c r="S229" s="0" t="n">
-        <f aca="false">IF(AND(R229="no", E229="tertiary"),-N229,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R229="no", E229="secondary"),-N229,0)</f>
+        <v>-3</v>
       </c>
       <c r="T229" s="0" t="n">
-        <f aca="false">IF(AND(R229="yes", E229="tertiary"),11-N229,0)</f>
+        <f aca="false">IF(AND(R229="yes", E229="secondary"),11-N229,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -14973,11 +14973,11 @@
         <v>22</v>
       </c>
       <c r="S230" s="0" t="n">
-        <f aca="false">IF(AND(R230="no", E230="tertiary"),-N230,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R230="no", E230="secondary"),-N230,0)</f>
+        <v>-2</v>
       </c>
       <c r="T230" s="0" t="n">
-        <f aca="false">IF(AND(R230="yes", E230="tertiary"),11-N230,0)</f>
+        <f aca="false">IF(AND(R230="yes", E230="secondary"),11-N230,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15037,11 +15037,11 @@
         <v>22</v>
       </c>
       <c r="S231" s="0" t="n">
-        <f aca="false">IF(AND(R231="no", E231="tertiary"),-N231,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R231="no", E231="secondary"),-N231,0)</f>
+        <v>-1</v>
       </c>
       <c r="T231" s="0" t="n">
-        <f aca="false">IF(AND(R231="yes", E231="tertiary"),11-N231,0)</f>
+        <f aca="false">IF(AND(R231="yes", E231="secondary"),11-N231,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15101,11 +15101,11 @@
         <v>22</v>
       </c>
       <c r="S232" s="0" t="n">
-        <f aca="false">IF(AND(R232="no", E232="tertiary"),-N232,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R232="no", E232="secondary"),-N232,0)</f>
+        <v>-2</v>
       </c>
       <c r="T232" s="0" t="n">
-        <f aca="false">IF(AND(R232="yes", E232="tertiary"),11-N232,0)</f>
+        <f aca="false">IF(AND(R232="yes", E232="secondary"),11-N232,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15165,11 +15165,11 @@
         <v>22</v>
       </c>
       <c r="S233" s="0" t="n">
-        <f aca="false">IF(AND(R233="no", E233="tertiary"),-N233,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R233="no", E233="secondary"),-N233,0)</f>
+        <v>-2</v>
       </c>
       <c r="T233" s="0" t="n">
-        <f aca="false">IF(AND(R233="yes", E233="tertiary"),11-N233,0)</f>
+        <f aca="false">IF(AND(R233="yes", E233="secondary"),11-N233,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15229,11 +15229,11 @@
         <v>22</v>
       </c>
       <c r="S234" s="0" t="n">
-        <f aca="false">IF(AND(R234="no", E234="tertiary"),-N234,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R234="no", E234="secondary"),-N234,0)</f>
+        <v>0</v>
       </c>
       <c r="T234" s="0" t="n">
-        <f aca="false">IF(AND(R234="yes", E234="tertiary"),11-N234,0)</f>
+        <f aca="false">IF(AND(R234="yes", E234="secondary"),11-N234,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15293,11 +15293,11 @@
         <v>22</v>
       </c>
       <c r="S235" s="0" t="n">
-        <f aca="false">IF(AND(R235="no", E235="tertiary"),-N235,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R235="no", E235="secondary"),-N235,0)</f>
+        <v>-1</v>
       </c>
       <c r="T235" s="0" t="n">
-        <f aca="false">IF(AND(R235="yes", E235="tertiary"),11-N235,0)</f>
+        <f aca="false">IF(AND(R235="yes", E235="secondary"),11-N235,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15357,11 +15357,11 @@
         <v>22</v>
       </c>
       <c r="S236" s="0" t="n">
-        <f aca="false">IF(AND(R236="no", E236="tertiary"),-N236,0)</f>
-        <v>-3</v>
+        <f aca="false">IF(AND(R236="no", E236="secondary"),-N236,0)</f>
+        <v>0</v>
       </c>
       <c r="T236" s="0" t="n">
-        <f aca="false">IF(AND(R236="yes", E236="tertiary"),11-N236,0)</f>
+        <f aca="false">IF(AND(R236="yes", E236="secondary"),11-N236,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15421,11 +15421,11 @@
         <v>22</v>
       </c>
       <c r="S237" s="0" t="n">
-        <f aca="false">IF(AND(R237="no", E237="tertiary"),-N237,0)</f>
+        <f aca="false">IF(AND(R237="no", E237="secondary"),-N237,0)</f>
         <v>0</v>
       </c>
       <c r="T237" s="0" t="n">
-        <f aca="false">IF(AND(R237="yes", E237="tertiary"),11-N237,0)</f>
+        <f aca="false">IF(AND(R237="yes", E237="secondary"),11-N237,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15485,11 +15485,11 @@
         <v>22</v>
       </c>
       <c r="S238" s="0" t="n">
-        <f aca="false">IF(AND(R238="no", E238="tertiary"),-N238,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R238="no", E238="secondary"),-N238,0)</f>
+        <v>0</v>
       </c>
       <c r="T238" s="0" t="n">
-        <f aca="false">IF(AND(R238="yes", E238="tertiary"),11-N238,0)</f>
+        <f aca="false">IF(AND(R238="yes", E238="secondary"),11-N238,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15549,11 +15549,11 @@
         <v>22</v>
       </c>
       <c r="S239" s="0" t="n">
-        <f aca="false">IF(AND(R239="no", E239="tertiary"),-N239,0)</f>
-        <v>-1</v>
+        <f aca="false">IF(AND(R239="no", E239="secondary"),-N239,0)</f>
+        <v>0</v>
       </c>
       <c r="T239" s="0" t="n">
-        <f aca="false">IF(AND(R239="yes", E239="tertiary"),11-N239,0)</f>
+        <f aca="false">IF(AND(R239="yes", E239="secondary"),11-N239,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15613,11 +15613,11 @@
         <v>22</v>
       </c>
       <c r="S240" s="0" t="n">
-        <f aca="false">IF(AND(R240="no", E240="tertiary"),-N240,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R240="no", E240="secondary"),-N240,0)</f>
+        <v>-2</v>
       </c>
       <c r="T240" s="0" t="n">
-        <f aca="false">IF(AND(R240="yes", E240="tertiary"),11-N240,0)</f>
+        <f aca="false">IF(AND(R240="yes", E240="secondary"),11-N240,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15677,11 +15677,11 @@
         <v>22</v>
       </c>
       <c r="S241" s="0" t="n">
-        <f aca="false">IF(AND(R241="no", E241="tertiary"),-N241,0)</f>
+        <f aca="false">IF(AND(R241="no", E241="secondary"),-N241,0)</f>
         <v>0</v>
       </c>
       <c r="T241" s="0" t="n">
-        <f aca="false">IF(AND(R241="yes", E241="tertiary"),11-N241,0)</f>
+        <f aca="false">IF(AND(R241="yes", E241="secondary"),11-N241,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15741,11 +15741,11 @@
         <v>22</v>
       </c>
       <c r="S242" s="0" t="n">
-        <f aca="false">IF(AND(R242="no", E242="tertiary"),-N242,0)</f>
+        <f aca="false">IF(AND(R242="no", E242="secondary"),-N242,0)</f>
         <v>0</v>
       </c>
       <c r="T242" s="0" t="n">
-        <f aca="false">IF(AND(R242="yes", E242="tertiary"),11-N242,0)</f>
+        <f aca="false">IF(AND(R242="yes", E242="secondary"),11-N242,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15805,12 +15805,12 @@
         <v>23</v>
       </c>
       <c r="S243" s="0" t="n">
-        <f aca="false">IF(AND(R243="no", E243="tertiary"),-N243,0)</f>
+        <f aca="false">IF(AND(R243="no", E243="secondary"),-N243,0)</f>
         <v>0</v>
       </c>
       <c r="T243" s="0" t="n">
-        <f aca="false">IF(AND(R243="yes", E243="tertiary"),11-N243,0)</f>
-        <v>9</v>
+        <f aca="false">IF(AND(R243="yes", E243="secondary"),11-N243,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15869,11 +15869,11 @@
         <v>22</v>
       </c>
       <c r="S244" s="0" t="n">
-        <f aca="false">IF(AND(R244="no", E244="tertiary"),-N244,0)</f>
+        <f aca="false">IF(AND(R244="no", E244="secondary"),-N244,0)</f>
         <v>0</v>
       </c>
       <c r="T244" s="0" t="n">
-        <f aca="false">IF(AND(R244="yes", E244="tertiary"),11-N244,0)</f>
+        <f aca="false">IF(AND(R244="yes", E244="secondary"),11-N244,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15933,11 +15933,11 @@
         <v>22</v>
       </c>
       <c r="S245" s="0" t="n">
-        <f aca="false">IF(AND(R245="no", E245="tertiary"),-N245,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R245="no", E245="secondary"),-N245,0)</f>
+        <v>-4</v>
       </c>
       <c r="T245" s="0" t="n">
-        <f aca="false">IF(AND(R245="yes", E245="tertiary"),11-N245,0)</f>
+        <f aca="false">IF(AND(R245="yes", E245="secondary"),11-N245,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -15997,11 +15997,11 @@
         <v>22</v>
       </c>
       <c r="S246" s="0" t="n">
-        <f aca="false">IF(AND(R246="no", E246="tertiary"),-N246,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R246="no", E246="secondary"),-N246,0)</f>
+        <v>-3</v>
       </c>
       <c r="T246" s="0" t="n">
-        <f aca="false">IF(AND(R246="yes", E246="tertiary"),11-N246,0)</f>
+        <f aca="false">IF(AND(R246="yes", E246="secondary"),11-N246,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16061,11 +16061,11 @@
         <v>22</v>
       </c>
       <c r="S247" s="0" t="n">
-        <f aca="false">IF(AND(R247="no", E247="tertiary"),-N247,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R247="no", E247="secondary"),-N247,0)</f>
+        <v>-2</v>
       </c>
       <c r="T247" s="0" t="n">
-        <f aca="false">IF(AND(R247="yes", E247="tertiary"),11-N247,0)</f>
+        <f aca="false">IF(AND(R247="yes", E247="secondary"),11-N247,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16125,11 +16125,11 @@
         <v>22</v>
       </c>
       <c r="S248" s="0" t="n">
-        <f aca="false">IF(AND(R248="no", E248="tertiary"),-N248,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R248="no", E248="secondary"),-N248,0)</f>
+        <v>-3</v>
       </c>
       <c r="T248" s="0" t="n">
-        <f aca="false">IF(AND(R248="yes", E248="tertiary"),11-N248,0)</f>
+        <f aca="false">IF(AND(R248="yes", E248="secondary"),11-N248,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16189,11 +16189,11 @@
         <v>22</v>
       </c>
       <c r="S249" s="0" t="n">
-        <f aca="false">IF(AND(R249="no", E249="tertiary"),-N249,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R249="no", E249="secondary"),-N249,0)</f>
+        <v>-3</v>
       </c>
       <c r="T249" s="0" t="n">
-        <f aca="false">IF(AND(R249="yes", E249="tertiary"),11-N249,0)</f>
+        <f aca="false">IF(AND(R249="yes", E249="secondary"),11-N249,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16253,11 +16253,11 @@
         <v>22</v>
       </c>
       <c r="S250" s="0" t="n">
-        <f aca="false">IF(AND(R250="no", E250="tertiary"),-N250,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R250="no", E250="secondary"),-N250,0)</f>
+        <v>-2</v>
       </c>
       <c r="T250" s="0" t="n">
-        <f aca="false">IF(AND(R250="yes", E250="tertiary"),11-N250,0)</f>
+        <f aca="false">IF(AND(R250="yes", E250="secondary"),11-N250,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16317,11 +16317,11 @@
         <v>22</v>
       </c>
       <c r="S251" s="0" t="n">
-        <f aca="false">IF(AND(R251="no", E251="tertiary"),-N251,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R251="no", E251="secondary"),-N251,0)</f>
+        <v>-2</v>
       </c>
       <c r="T251" s="0" t="n">
-        <f aca="false">IF(AND(R251="yes", E251="tertiary"),11-N251,0)</f>
+        <f aca="false">IF(AND(R251="yes", E251="secondary"),11-N251,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16381,11 +16381,11 @@
         <v>22</v>
       </c>
       <c r="S252" s="0" t="n">
-        <f aca="false">IF(AND(R252="no", E252="tertiary"),-N252,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R252="no", E252="secondary"),-N252,0)</f>
+        <v>0</v>
       </c>
       <c r="T252" s="0" t="n">
-        <f aca="false">IF(AND(R252="yes", E252="tertiary"),11-N252,0)</f>
+        <f aca="false">IF(AND(R252="yes", E252="secondary"),11-N252,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16445,11 +16445,11 @@
         <v>22</v>
       </c>
       <c r="S253" s="0" t="n">
-        <f aca="false">IF(AND(R253="no", E253="tertiary"),-N253,0)</f>
+        <f aca="false">IF(AND(R253="no", E253="secondary"),-N253,0)</f>
         <v>0</v>
       </c>
       <c r="T253" s="0" t="n">
-        <f aca="false">IF(AND(R253="yes", E253="tertiary"),11-N253,0)</f>
+        <f aca="false">IF(AND(R253="yes", E253="secondary"),11-N253,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16509,11 +16509,11 @@
         <v>22</v>
       </c>
       <c r="S254" s="0" t="n">
-        <f aca="false">IF(AND(R254="no", E254="tertiary"),-N254,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R254="no", E254="secondary"),-N254,0)</f>
+        <v>-2</v>
       </c>
       <c r="T254" s="0" t="n">
-        <f aca="false">IF(AND(R254="yes", E254="tertiary"),11-N254,0)</f>
+        <f aca="false">IF(AND(R254="yes", E254="secondary"),11-N254,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16573,11 +16573,11 @@
         <v>22</v>
       </c>
       <c r="S255" s="0" t="n">
-        <f aca="false">IF(AND(R255="no", E255="tertiary"),-N255,0)</f>
-        <v>-4</v>
+        <f aca="false">IF(AND(R255="no", E255="secondary"),-N255,0)</f>
+        <v>0</v>
       </c>
       <c r="T255" s="0" t="n">
-        <f aca="false">IF(AND(R255="yes", E255="tertiary"),11-N255,0)</f>
+        <f aca="false">IF(AND(R255="yes", E255="secondary"),11-N255,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16637,11 +16637,11 @@
         <v>22</v>
       </c>
       <c r="S256" s="0" t="n">
-        <f aca="false">IF(AND(R256="no", E256="tertiary"),-N256,0)</f>
+        <f aca="false">IF(AND(R256="no", E256="secondary"),-N256,0)</f>
         <v>0</v>
       </c>
       <c r="T256" s="0" t="n">
-        <f aca="false">IF(AND(R256="yes", E256="tertiary"),11-N256,0)</f>
+        <f aca="false">IF(AND(R256="yes", E256="secondary"),11-N256,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16701,11 +16701,11 @@
         <v>22</v>
       </c>
       <c r="S257" s="0" t="n">
-        <f aca="false">IF(AND(R257="no", E257="tertiary"),-N257,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R257="no", E257="secondary"),-N257,0)</f>
+        <v>-2</v>
       </c>
       <c r="T257" s="0" t="n">
-        <f aca="false">IF(AND(R257="yes", E257="tertiary"),11-N257,0)</f>
+        <f aca="false">IF(AND(R257="yes", E257="secondary"),11-N257,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16765,11 +16765,11 @@
         <v>22</v>
       </c>
       <c r="S258" s="0" t="n">
-        <f aca="false">IF(AND(R258="no", E258="tertiary"),-N258,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R258="no", E258="secondary"),-N258,0)</f>
+        <v>-2</v>
       </c>
       <c r="T258" s="0" t="n">
-        <f aca="false">IF(AND(R258="yes", E258="tertiary"),11-N258,0)</f>
+        <f aca="false">IF(AND(R258="yes", E258="secondary"),11-N258,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16829,11 +16829,11 @@
         <v>22</v>
       </c>
       <c r="S259" s="0" t="n">
-        <f aca="false">IF(AND(R259="no", E259="tertiary"),-N259,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R259="no", E259="secondary"),-N259,0)</f>
+        <v>-2</v>
       </c>
       <c r="T259" s="0" t="n">
-        <f aca="false">IF(AND(R259="yes", E259="tertiary"),11-N259,0)</f>
+        <f aca="false">IF(AND(R259="yes", E259="secondary"),11-N259,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16893,11 +16893,11 @@
         <v>22</v>
       </c>
       <c r="S260" s="0" t="n">
-        <f aca="false">IF(AND(R260="no", E260="tertiary"),-N260,0)</f>
-        <v>-3</v>
+        <f aca="false">IF(AND(R260="no", E260="secondary"),-N260,0)</f>
+        <v>0</v>
       </c>
       <c r="T260" s="0" t="n">
-        <f aca="false">IF(AND(R260="yes", E260="tertiary"),11-N260,0)</f>
+        <f aca="false">IF(AND(R260="yes", E260="secondary"),11-N260,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -16957,11 +16957,11 @@
         <v>22</v>
       </c>
       <c r="S261" s="0" t="n">
-        <f aca="false">IF(AND(R261="no", E261="tertiary"),-N261,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R261="no", E261="secondary"),-N261,0)</f>
+        <v>-2</v>
       </c>
       <c r="T261" s="0" t="n">
-        <f aca="false">IF(AND(R261="yes", E261="tertiary"),11-N261,0)</f>
+        <f aca="false">IF(AND(R261="yes", E261="secondary"),11-N261,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17021,11 +17021,11 @@
         <v>22</v>
       </c>
       <c r="S262" s="0" t="n">
-        <f aca="false">IF(AND(R262="no", E262="tertiary"),-N262,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R262="no", E262="secondary"),-N262,0)</f>
+        <v>-2</v>
       </c>
       <c r="T262" s="0" t="n">
-        <f aca="false">IF(AND(R262="yes", E262="tertiary"),11-N262,0)</f>
+        <f aca="false">IF(AND(R262="yes", E262="secondary"),11-N262,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17085,11 +17085,11 @@
         <v>22</v>
       </c>
       <c r="S263" s="0" t="n">
-        <f aca="false">IF(AND(R263="no", E263="tertiary"),-N263,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R263="no", E263="secondary"),-N263,0)</f>
+        <v>0</v>
       </c>
       <c r="T263" s="0" t="n">
-        <f aca="false">IF(AND(R263="yes", E263="tertiary"),11-N263,0)</f>
+        <f aca="false">IF(AND(R263="yes", E263="secondary"),11-N263,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17149,11 +17149,11 @@
         <v>22</v>
       </c>
       <c r="S264" s="0" t="n">
-        <f aca="false">IF(AND(R264="no", E264="tertiary"),-N264,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R264="no", E264="secondary"),-N264,0)</f>
+        <v>-3</v>
       </c>
       <c r="T264" s="0" t="n">
-        <f aca="false">IF(AND(R264="yes", E264="tertiary"),11-N264,0)</f>
+        <f aca="false">IF(AND(R264="yes", E264="secondary"),11-N264,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17213,11 +17213,11 @@
         <v>22</v>
       </c>
       <c r="S265" s="0" t="n">
-        <f aca="false">IF(AND(R265="no", E265="tertiary"),-N265,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R265="no", E265="secondary"),-N265,0)</f>
+        <v>0</v>
       </c>
       <c r="T265" s="0" t="n">
-        <f aca="false">IF(AND(R265="yes", E265="tertiary"),11-N265,0)</f>
+        <f aca="false">IF(AND(R265="yes", E265="secondary"),11-N265,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17277,11 +17277,11 @@
         <v>22</v>
       </c>
       <c r="S266" s="0" t="n">
-        <f aca="false">IF(AND(R266="no", E266="tertiary"),-N266,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R266="no", E266="secondary"),-N266,0)</f>
+        <v>-4</v>
       </c>
       <c r="T266" s="0" t="n">
-        <f aca="false">IF(AND(R266="yes", E266="tertiary"),11-N266,0)</f>
+        <f aca="false">IF(AND(R266="yes", E266="secondary"),11-N266,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17341,11 +17341,11 @@
         <v>22</v>
       </c>
       <c r="S267" s="0" t="n">
-        <f aca="false">IF(AND(R267="no", E267="tertiary"),-N267,0)</f>
+        <f aca="false">IF(AND(R267="no", E267="secondary"),-N267,0)</f>
         <v>0</v>
       </c>
       <c r="T267" s="0" t="n">
-        <f aca="false">IF(AND(R267="yes", E267="tertiary"),11-N267,0)</f>
+        <f aca="false">IF(AND(R267="yes", E267="secondary"),11-N267,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17405,11 +17405,11 @@
         <v>22</v>
       </c>
       <c r="S268" s="0" t="n">
-        <f aca="false">IF(AND(R268="no", E268="tertiary"),-N268,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R268="no", E268="secondary"),-N268,0)</f>
+        <v>-2</v>
       </c>
       <c r="T268" s="0" t="n">
-        <f aca="false">IF(AND(R268="yes", E268="tertiary"),11-N268,0)</f>
+        <f aca="false">IF(AND(R268="yes", E268="secondary"),11-N268,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17469,11 +17469,11 @@
         <v>22</v>
       </c>
       <c r="S269" s="0" t="n">
-        <f aca="false">IF(AND(R269="no", E269="tertiary"),-N269,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R269="no", E269="secondary"),-N269,0)</f>
+        <v>-2</v>
       </c>
       <c r="T269" s="0" t="n">
-        <f aca="false">IF(AND(R269="yes", E269="tertiary"),11-N269,0)</f>
+        <f aca="false">IF(AND(R269="yes", E269="secondary"),11-N269,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17533,11 +17533,11 @@
         <v>22</v>
       </c>
       <c r="S270" s="0" t="n">
-        <f aca="false">IF(AND(R270="no", E270="tertiary"),-N270,0)</f>
+        <f aca="false">IF(AND(R270="no", E270="secondary"),-N270,0)</f>
         <v>0</v>
       </c>
       <c r="T270" s="0" t="n">
-        <f aca="false">IF(AND(R270="yes", E270="tertiary"),11-N270,0)</f>
+        <f aca="false">IF(AND(R270="yes", E270="secondary"),11-N270,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17597,11 +17597,11 @@
         <v>22</v>
       </c>
       <c r="S271" s="0" t="n">
-        <f aca="false">IF(AND(R271="no", E271="tertiary"),-N271,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R271="no", E271="secondary"),-N271,0)</f>
+        <v>-2</v>
       </c>
       <c r="T271" s="0" t="n">
-        <f aca="false">IF(AND(R271="yes", E271="tertiary"),11-N271,0)</f>
+        <f aca="false">IF(AND(R271="yes", E271="secondary"),11-N271,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17661,11 +17661,11 @@
         <v>22</v>
       </c>
       <c r="S272" s="0" t="n">
-        <f aca="false">IF(AND(R272="no", E272="tertiary"),-N272,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R272="no", E272="secondary"),-N272,0)</f>
+        <v>-2</v>
       </c>
       <c r="T272" s="0" t="n">
-        <f aca="false">IF(AND(R272="yes", E272="tertiary"),11-N272,0)</f>
+        <f aca="false">IF(AND(R272="yes", E272="secondary"),11-N272,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17725,11 +17725,11 @@
         <v>22</v>
       </c>
       <c r="S273" s="0" t="n">
-        <f aca="false">IF(AND(R273="no", E273="tertiary"),-N273,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R273="no", E273="secondary"),-N273,0)</f>
+        <v>-2</v>
       </c>
       <c r="T273" s="0" t="n">
-        <f aca="false">IF(AND(R273="yes", E273="tertiary"),11-N273,0)</f>
+        <f aca="false">IF(AND(R273="yes", E273="secondary"),11-N273,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17789,11 +17789,11 @@
         <v>22</v>
       </c>
       <c r="S274" s="0" t="n">
-        <f aca="false">IF(AND(R274="no", E274="tertiary"),-N274,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R274="no", E274="secondary"),-N274,0)</f>
+        <v>-2</v>
       </c>
       <c r="T274" s="0" t="n">
-        <f aca="false">IF(AND(R274="yes", E274="tertiary"),11-N274,0)</f>
+        <f aca="false">IF(AND(R274="yes", E274="secondary"),11-N274,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17853,11 +17853,11 @@
         <v>22</v>
       </c>
       <c r="S275" s="0" t="n">
-        <f aca="false">IF(AND(R275="no", E275="tertiary"),-N275,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R275="no", E275="secondary"),-N275,0)</f>
+        <v>-2</v>
       </c>
       <c r="T275" s="0" t="n">
-        <f aca="false">IF(AND(R275="yes", E275="tertiary"),11-N275,0)</f>
+        <f aca="false">IF(AND(R275="yes", E275="secondary"),11-N275,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17917,11 +17917,11 @@
         <v>22</v>
       </c>
       <c r="S276" s="0" t="n">
-        <f aca="false">IF(AND(R276="no", E276="tertiary"),-N276,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R276="no", E276="secondary"),-N276,0)</f>
+        <v>0</v>
       </c>
       <c r="T276" s="0" t="n">
-        <f aca="false">IF(AND(R276="yes", E276="tertiary"),11-N276,0)</f>
+        <f aca="false">IF(AND(R276="yes", E276="secondary"),11-N276,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -17981,11 +17981,11 @@
         <v>22</v>
       </c>
       <c r="S277" s="0" t="n">
-        <f aca="false">IF(AND(R277="no", E277="tertiary"),-N277,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R277="no", E277="secondary"),-N277,0)</f>
+        <v>-3</v>
       </c>
       <c r="T277" s="0" t="n">
-        <f aca="false">IF(AND(R277="yes", E277="tertiary"),11-N277,0)</f>
+        <f aca="false">IF(AND(R277="yes", E277="secondary"),11-N277,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18045,11 +18045,11 @@
         <v>22</v>
       </c>
       <c r="S278" s="0" t="n">
-        <f aca="false">IF(AND(R278="no", E278="tertiary"),-N278,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R278="no", E278="secondary"),-N278,0)</f>
+        <v>-2</v>
       </c>
       <c r="T278" s="0" t="n">
-        <f aca="false">IF(AND(R278="yes", E278="tertiary"),11-N278,0)</f>
+        <f aca="false">IF(AND(R278="yes", E278="secondary"),11-N278,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18109,11 +18109,11 @@
         <v>22</v>
       </c>
       <c r="S279" s="0" t="n">
-        <f aca="false">IF(AND(R279="no", E279="tertiary"),-N279,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R279="no", E279="secondary"),-N279,0)</f>
+        <v>-2</v>
       </c>
       <c r="T279" s="0" t="n">
-        <f aca="false">IF(AND(R279="yes", E279="tertiary"),11-N279,0)</f>
+        <f aca="false">IF(AND(R279="yes", E279="secondary"),11-N279,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18173,11 +18173,11 @@
         <v>22</v>
       </c>
       <c r="S280" s="0" t="n">
-        <f aca="false">IF(AND(R280="no", E280="tertiary"),-N280,0)</f>
+        <f aca="false">IF(AND(R280="no", E280="secondary"),-N280,0)</f>
         <v>0</v>
       </c>
       <c r="T280" s="0" t="n">
-        <f aca="false">IF(AND(R280="yes", E280="tertiary"),11-N280,0)</f>
+        <f aca="false">IF(AND(R280="yes", E280="secondary"),11-N280,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18237,11 +18237,11 @@
         <v>22</v>
       </c>
       <c r="S281" s="0" t="n">
-        <f aca="false">IF(AND(R281="no", E281="tertiary"),-N281,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R281="no", E281="secondary"),-N281,0)</f>
+        <v>-2</v>
       </c>
       <c r="T281" s="0" t="n">
-        <f aca="false">IF(AND(R281="yes", E281="tertiary"),11-N281,0)</f>
+        <f aca="false">IF(AND(R281="yes", E281="secondary"),11-N281,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18301,11 +18301,11 @@
         <v>22</v>
       </c>
       <c r="S282" s="0" t="n">
-        <f aca="false">IF(AND(R282="no", E282="tertiary"),-N282,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R282="no", E282="secondary"),-N282,0)</f>
+        <v>0</v>
       </c>
       <c r="T282" s="0" t="n">
-        <f aca="false">IF(AND(R282="yes", E282="tertiary"),11-N282,0)</f>
+        <f aca="false">IF(AND(R282="yes", E282="secondary"),11-N282,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18365,11 +18365,11 @@
         <v>22</v>
       </c>
       <c r="S283" s="0" t="n">
-        <f aca="false">IF(AND(R283="no", E283="tertiary"),-N283,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R283="no", E283="secondary"),-N283,0)</f>
+        <v>-2</v>
       </c>
       <c r="T283" s="0" t="n">
-        <f aca="false">IF(AND(R283="yes", E283="tertiary"),11-N283,0)</f>
+        <f aca="false">IF(AND(R283="yes", E283="secondary"),11-N283,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18429,11 +18429,11 @@
         <v>22</v>
       </c>
       <c r="S284" s="0" t="n">
-        <f aca="false">IF(AND(R284="no", E284="tertiary"),-N284,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R284="no", E284="secondary"),-N284,0)</f>
+        <v>-2</v>
       </c>
       <c r="T284" s="0" t="n">
-        <f aca="false">IF(AND(R284="yes", E284="tertiary"),11-N284,0)</f>
+        <f aca="false">IF(AND(R284="yes", E284="secondary"),11-N284,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18493,11 +18493,11 @@
         <v>22</v>
       </c>
       <c r="S285" s="0" t="n">
-        <f aca="false">IF(AND(R285="no", E285="tertiary"),-N285,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R285="no", E285="secondary"),-N285,0)</f>
+        <v>-2</v>
       </c>
       <c r="T285" s="0" t="n">
-        <f aca="false">IF(AND(R285="yes", E285="tertiary"),11-N285,0)</f>
+        <f aca="false">IF(AND(R285="yes", E285="secondary"),11-N285,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18557,11 +18557,11 @@
         <v>22</v>
       </c>
       <c r="S286" s="0" t="n">
-        <f aca="false">IF(AND(R286="no", E286="tertiary"),-N286,0)</f>
+        <f aca="false">IF(AND(R286="no", E286="secondary"),-N286,0)</f>
         <v>0</v>
       </c>
       <c r="T286" s="0" t="n">
-        <f aca="false">IF(AND(R286="yes", E286="tertiary"),11-N286,0)</f>
+        <f aca="false">IF(AND(R286="yes", E286="secondary"),11-N286,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18621,11 +18621,11 @@
         <v>22</v>
       </c>
       <c r="S287" s="0" t="n">
-        <f aca="false">IF(AND(R287="no", E287="tertiary"),-N287,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R287="no", E287="secondary"),-N287,0)</f>
+        <v>-2</v>
       </c>
       <c r="T287" s="0" t="n">
-        <f aca="false">IF(AND(R287="yes", E287="tertiary"),11-N287,0)</f>
+        <f aca="false">IF(AND(R287="yes", E287="secondary"),11-N287,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18685,11 +18685,11 @@
         <v>22</v>
       </c>
       <c r="S288" s="0" t="n">
-        <f aca="false">IF(AND(R288="no", E288="tertiary"),-N288,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R288="no", E288="secondary"),-N288,0)</f>
+        <v>-2</v>
       </c>
       <c r="T288" s="0" t="n">
-        <f aca="false">IF(AND(R288="yes", E288="tertiary"),11-N288,0)</f>
+        <f aca="false">IF(AND(R288="yes", E288="secondary"),11-N288,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18749,11 +18749,11 @@
         <v>22</v>
       </c>
       <c r="S289" s="0" t="n">
-        <f aca="false">IF(AND(R289="no", E289="tertiary"),-N289,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R289="no", E289="secondary"),-N289,0)</f>
+        <v>-3</v>
       </c>
       <c r="T289" s="0" t="n">
-        <f aca="false">IF(AND(R289="yes", E289="tertiary"),11-N289,0)</f>
+        <f aca="false">IF(AND(R289="yes", E289="secondary"),11-N289,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18813,11 +18813,11 @@
         <v>22</v>
       </c>
       <c r="S290" s="0" t="n">
-        <f aca="false">IF(AND(R290="no", E290="tertiary"),-N290,0)</f>
-        <v>-2</v>
+        <f aca="false">IF(AND(R290="no", E290="secondary"),-N290,0)</f>
+        <v>0</v>
       </c>
       <c r="T290" s="0" t="n">
-        <f aca="false">IF(AND(R290="yes", E290="tertiary"),11-N290,0)</f>
+        <f aca="false">IF(AND(R290="yes", E290="secondary"),11-N290,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18877,11 +18877,11 @@
         <v>22</v>
       </c>
       <c r="S291" s="0" t="n">
-        <f aca="false">IF(AND(R291="no", E291="tertiary"),-N291,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R291="no", E291="secondary"),-N291,0)</f>
+        <v>-2</v>
       </c>
       <c r="T291" s="0" t="n">
-        <f aca="false">IF(AND(R291="yes", E291="tertiary"),11-N291,0)</f>
+        <f aca="false">IF(AND(R291="yes", E291="secondary"),11-N291,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18941,11 +18941,11 @@
         <v>22</v>
       </c>
       <c r="S292" s="0" t="n">
-        <f aca="false">IF(AND(R292="no", E292="tertiary"),-N292,0)</f>
-        <v>-4</v>
+        <f aca="false">IF(AND(R292="no", E292="secondary"),-N292,0)</f>
+        <v>0</v>
       </c>
       <c r="T292" s="0" t="n">
-        <f aca="false">IF(AND(R292="yes", E292="tertiary"),11-N292,0)</f>
+        <f aca="false">IF(AND(R292="yes", E292="secondary"),11-N292,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19005,11 +19005,11 @@
         <v>22</v>
       </c>
       <c r="S293" s="0" t="n">
-        <f aca="false">IF(AND(R293="no", E293="tertiary"),-N293,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R293="no", E293="secondary"),-N293,0)</f>
+        <v>-3</v>
       </c>
       <c r="T293" s="0" t="n">
-        <f aca="false">IF(AND(R293="yes", E293="tertiary"),11-N293,0)</f>
+        <f aca="false">IF(AND(R293="yes", E293="secondary"),11-N293,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19069,11 +19069,11 @@
         <v>22</v>
       </c>
       <c r="S294" s="0" t="n">
-        <f aca="false">IF(AND(R294="no", E294="tertiary"),-N294,0)</f>
-        <v>-3</v>
+        <f aca="false">IF(AND(R294="no", E294="secondary"),-N294,0)</f>
+        <v>0</v>
       </c>
       <c r="T294" s="0" t="n">
-        <f aca="false">IF(AND(R294="yes", E294="tertiary"),11-N294,0)</f>
+        <f aca="false">IF(AND(R294="yes", E294="secondary"),11-N294,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19133,11 +19133,11 @@
         <v>22</v>
       </c>
       <c r="S295" s="0" t="n">
-        <f aca="false">IF(AND(R295="no", E295="tertiary"),-N295,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R295="no", E295="secondary"),-N295,0)</f>
+        <v>-2</v>
       </c>
       <c r="T295" s="0" t="n">
-        <f aca="false">IF(AND(R295="yes", E295="tertiary"),11-N295,0)</f>
+        <f aca="false">IF(AND(R295="yes", E295="secondary"),11-N295,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19197,11 +19197,11 @@
         <v>22</v>
       </c>
       <c r="S296" s="0" t="n">
-        <f aca="false">IF(AND(R296="no", E296="tertiary"),-N296,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R296="no", E296="secondary"),-N296,0)</f>
+        <v>-3</v>
       </c>
       <c r="T296" s="0" t="n">
-        <f aca="false">IF(AND(R296="yes", E296="tertiary"),11-N296,0)</f>
+        <f aca="false">IF(AND(R296="yes", E296="secondary"),11-N296,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19261,11 +19261,11 @@
         <v>22</v>
       </c>
       <c r="S297" s="0" t="n">
-        <f aca="false">IF(AND(R297="no", E297="tertiary"),-N297,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R297="no", E297="secondary"),-N297,0)</f>
+        <v>-2</v>
       </c>
       <c r="T297" s="0" t="n">
-        <f aca="false">IF(AND(R297="yes", E297="tertiary"),11-N297,0)</f>
+        <f aca="false">IF(AND(R297="yes", E297="secondary"),11-N297,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19325,11 +19325,11 @@
         <v>22</v>
       </c>
       <c r="S298" s="0" t="n">
-        <f aca="false">IF(AND(R298="no", E298="tertiary"),-N298,0)</f>
-        <v>-5</v>
+        <f aca="false">IF(AND(R298="no", E298="secondary"),-N298,0)</f>
+        <v>0</v>
       </c>
       <c r="T298" s="0" t="n">
-        <f aca="false">IF(AND(R298="yes", E298="tertiary"),11-N298,0)</f>
+        <f aca="false">IF(AND(R298="yes", E298="secondary"),11-N298,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19389,11 +19389,11 @@
         <v>22</v>
       </c>
       <c r="S299" s="0" t="n">
-        <f aca="false">IF(AND(R299="no", E299="tertiary"),-N299,0)</f>
-        <v>-3</v>
+        <f aca="false">IF(AND(R299="no", E299="secondary"),-N299,0)</f>
+        <v>0</v>
       </c>
       <c r="T299" s="0" t="n">
-        <f aca="false">IF(AND(R299="yes", E299="tertiary"),11-N299,0)</f>
+        <f aca="false">IF(AND(R299="yes", E299="secondary"),11-N299,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19453,11 +19453,11 @@
         <v>22</v>
       </c>
       <c r="S300" s="0" t="n">
-        <f aca="false">IF(AND(R300="no", E300="tertiary"),-N300,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R300="no", E300="secondary"),-N300,0)</f>
+        <v>-4</v>
       </c>
       <c r="T300" s="0" t="n">
-        <f aca="false">IF(AND(R300="yes", E300="tertiary"),11-N300,0)</f>
+        <f aca="false">IF(AND(R300="yes", E300="secondary"),11-N300,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19517,40 +19517,40 @@
         <v>22</v>
       </c>
       <c r="S301" s="0" t="n">
-        <f aca="false">IF(AND(R301="no", E301="tertiary"),-N301,0)</f>
-        <v>0</v>
+        <f aca="false">IF(AND(R301="no", E301="secondary"),-N301,0)</f>
+        <v>-2</v>
       </c>
       <c r="T301" s="0" t="n">
-        <f aca="false">IF(AND(R301="yes", E301="tertiary"),11-N301,0)</f>
+        <f aca="false">IF(AND(R301="yes", E301="secondary"),11-N301,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S302" s="0" t="n">
         <f aca="false">SUM(S2:S301)</f>
-        <v>-98</v>
+        <v>-273</v>
       </c>
       <c r="T302" s="0" t="n">
         <f aca="false">SUM(T2:T301)</f>
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S303" s="0" t="n">
         <f aca="false">S302+T302</f>
-        <v>-80</v>
+        <v>-233</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S307" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E301,"tertiary")</f>
-        <v>67</v>
+        <f aca="false">COUNTIF(E2:E301,"secondary")</f>
+        <v>185</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S310" s="0" t="n">
         <f aca="false">S303/S307</f>
-        <v>-1.19402985074627</v>
+        <v>-1.25945945945946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>